<commit_message>
had added a few duplicate checks. I think Genelle thought they weren't there because they had different text.
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="233">
   <si>
     <t>Source</t>
   </si>
@@ -85,7 +85,7 @@
     <t>file structure</t>
   </si>
   <si>
-    <t>Nulls or incorrect data type</t>
+    <t>Nulls not allowed or incorrect data type</t>
   </si>
   <si>
     <t>Specific data elements will be identified in the Detail column of a CoC&amp;apos;s Integrity Checks export.</t>
@@ -115,7 +115,7 @@
     <t>EnrollmentIDs should be unique in the Enrollment file. There may be no more than one record for any PersonalID with the same EnrollmentID. If there is more than one record for the same PersonalID with the same EnrollmentID, this represents an error in the CSV export algorithm.</t>
   </si>
   <si>
-    <t>Client in the Enrollment file not found in Client file</t>
+    <t>PersonalID missing from Client.csv</t>
   </si>
   <si>
     <t>Per the HMIS CSV Format Specifications, all PersonalIDs in the Enrollment file should have a record in the Client file.</t>
@@ -605,10 +605,115 @@
     <t>Any project with active beds in the reporting period should have one or more active clients in the reporting period.</t>
   </si>
   <si>
+    <t>Incorrect DOB or Entry Date</t>
+  </si>
+  <si>
+    <t>The HMIS data is indicating the client entered the project PRIOR to being born. Correct either the Date of Birth or the Project Start Date,  whichever is incorrect.</t>
+  </si>
+  <si>
+    <t>Missing SSN</t>
+  </si>
+  <si>
+    <t>This data element is required to be collected at Project Start. Please go to the client's assessment at Project Start to enter this data to HMIS. If this data was not collected because the client declined to provide the information or was unable to provide it, please update the SSN Quality field accordingly</t>
+  </si>
+  <si>
+    <t>Oldest Household Member Under 12</t>
+  </si>
+  <si>
+    <t>This household has no one over the age of 12. This is unexpected and it could be an error. Please confirm date(s) of birth and household composition to ensure all members of the household are associated.</t>
+  </si>
+  <si>
+    <t>Income Missing at Entry</t>
+  </si>
+  <si>
+    <t>This data element is required to be collected at Project Start. Please go to the client's assessment at Project Start to enter this data to HMIS.</t>
+  </si>
+  <si>
+    <t>Conflicting Income yes/no at Entry</t>
+  </si>
+  <si>
+    <t>There is a discrepancy between the data element indicating that the client is receiving income and the data elements regarding the income sources. Please verify this client's income to correct this error.</t>
+  </si>
+  <si>
+    <t>Income Missing at Exit</t>
+  </si>
+  <si>
+    <t>This data element is required to be collected at Project Exit. Please go to the client's assessment at Project Exit to enter this data to HMIS.</t>
+  </si>
+  <si>
+    <t>Conflicting Income yes/no at Exit</t>
+  </si>
+  <si>
+    <t>Exit After Project's Operating End Date</t>
+  </si>
+  <si>
+    <t>This enrollment is active outside of the project's operating start and end dates. Please reconcile this by either correcting the enrollment dates or the project's operating dates.</t>
+  </si>
+  <si>
+    <t>Health Insurance Missing at Entry</t>
+  </si>
+  <si>
+    <t>Health Insurance Missing at Exit</t>
+  </si>
+  <si>
+    <t>Conflicting Health Insurance yes/no at Entry</t>
+  </si>
+  <si>
+    <t>There is a discrepancy between the data element indicating that the client is receiving health insurance and the data elements regarding the health insurance sources. Please verify this client's health insurance to correct this error.</t>
+  </si>
+  <si>
+    <t>Conflicting Health Insurance yes/no at Exit</t>
+  </si>
+  <si>
+    <t>Non-cash Benefits Missing at Entry</t>
+  </si>
+  <si>
+    <t>Conflicting Non-cash Benefits yes/no at Entry</t>
+  </si>
+  <si>
+    <t>There is a discrepancy between the data element indicating that the client is receiving non-cash benefits and the data elements regarding the non-cash benefits sources. Please verify this client's non-cash benefits to correct this error.</t>
+  </si>
+  <si>
+    <t>HouseholdID not incrementing correctly</t>
+  </si>
+  <si>
+    <t>The HouseholdID must be unique to the household stay in a project; reuse of the identification of the same or similar household upon readmission into the project is not permitted. Please review the HMIS Data Standards for more details.</t>
+  </si>
+  <si>
+    <t>Project Exit Before Start</t>
+  </si>
+  <si>
+    <t>This enrollment's exit date is before the enrollment's project start date. The exit date must be after the project start date. Please go to this enrollment and ensure that the correct project start date and exit date are entered.</t>
+  </si>
+  <si>
+    <t>Days Referral Active Exceeds Local Settings</t>
+  </si>
+  <si>
+    <t>You have at least one active referral that has been active without a Result Date for longer than the days set in your Local Settings on the Home tab.</t>
+  </si>
+  <si>
+    <t>No enrollment records</t>
+  </si>
+  <si>
+    <t>Your export's Enrollment.csv has 0 records. Without any enrollment data, Eva will not return any results on most analyses. If you are not sure how to run your HMIS CSV Export correctly, please contact your vendor.</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>The HMIS data is indicating the client entered the project PRIOR to being born. Correct either the Date of Birth or the Project Start Date, whichever is incorrect.</t>
+  </si>
+  <si>
+    <t>Nulls or incorrect data type</t>
+  </si>
+  <si>
     <t>Duplicate PersonalIDs found in the Client file</t>
   </si>
   <si>
     <t>Duplicate EnrollmentIDs found in the Enrollment file</t>
+  </si>
+  <si>
+    <t>Client in the Enrollment file not found in Client file</t>
   </si>
   <si>
     <t>ProjectID in the Enrollment file not found in Project file</t>
@@ -648,9 +753,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -964,12 +1072,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1000,7 +1108,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>228</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>23</v>
@@ -1020,7 +1128,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>195</v>
+        <v>229</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -1038,7 +1146,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>30</v>
@@ -1056,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
@@ -1074,7 +1182,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>35</v>
@@ -1358,12 +1466,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1586,12 +1694,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2618,18 +2726,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="44.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="60.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="44.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="60.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -4180,6 +4288,312 @@
       </c>
       <c r="F85" s="1"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+      <c r="A86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F86" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+      <c r="A87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F87" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+      <c r="A88" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F88" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+      <c r="A89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F89" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+      <c r="A90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F90" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+      <c r="A91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F91" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+      <c r="A92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F92" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+      <c r="A93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F93" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+      <c r="A94" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F94" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+      <c r="A95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F95" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+      <c r="A96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F96" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+      <c r="A97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F97" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+      <c r="A98" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F98" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+      <c r="A99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F99" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+      <c r="A100" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F100" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+      <c r="A101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F101" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+      <c r="A102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F102" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+      <c r="A103" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F103" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+      <c r="A104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F104" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
final additions to the All Checks tab (not sure what they are but git thinks they are different)
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="232">
   <si>
     <t>Source</t>
   </si>
@@ -696,9 +696,6 @@
   </si>
   <si>
     <t>Your export's Enrollment.csv has 0 records. Without any enrollment data, Eva will not return any results on most analyses. If you are not sure how to run your HMIS CSV Export correctly, please contact your vendor.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>The HMIS data is indicating the client entered the project PRIOR to being born. Correct either the Date of Birth or the Project Start Date, whichever is incorrect.</t>
@@ -753,12 +750,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1072,12 +1066,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1108,7 +1102,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>23</v>
@@ -1128,7 +1122,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -1146,7 +1140,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>30</v>
@@ -1164,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
@@ -1182,7 +1176,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>35</v>
@@ -1466,12 +1460,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1694,12 +1688,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2732,12 +2726,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="44.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="60.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="44.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="60.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -4586,11 +4580,9 @@
       <c r="C104" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="1"/>
+      <c r="E104" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="F104" s="1"/>
     </row>

</xml_diff>

<commit_message>
updated sandbox with latest app checks code
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="243">
   <si>
     <t>Source</t>
   </si>
@@ -742,6 +742,18 @@
   </si>
   <si>
     <t>3.10 - Project Start Date, 3.917.3 - Prior Living Situation: Date  Homelessness Started</t>
+  </si>
+  <si>
+    <t>Long Stayers</t>
+  </si>
+  <si>
+    <t>The number of days between Entry and the end of your CSV export exceeds the number of days in the Long Stayers settings for this project type. If this household has left the project, enter the Project Exit Date. If they are still active, do not change the data, but verify that your Coordinated Entry process is actively connecting this household to a permanent housing destination.</t>
+  </si>
+  <si>
+    <t>Days since Most Recent CLS Exceeds Local Settings</t>
+  </si>
+  <si>
+    <t>This enrollment has been active without any updates to their Current Living Situation for longer than the days set for this Project Type in your Long Stayers settings on the Edit Local Settings tab. Please be sure that any CLS updates or project exits are reflected in HMIS.</t>
   </si>
 </sst>
 </file>
@@ -3364,10 +3376,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5538,8 +5550,43 @@
         <v>101</v>
       </c>
     </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G104">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G102"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
for some reason not all changes had been saved. overwriting with changes to text that Genelle and Jesse made in early Aug
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="238">
   <si>
     <t>Source</t>
   </si>
@@ -739,9 +739,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>3.10 - Project Start Date, 3.917.3 - Prior Living Situation: Date  Homelessness Started</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1140,7 @@
         <v>175</v>
       </c>
       <c r="G2">
-        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$102,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$200,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>6</v>
       </c>
     </row>
@@ -1164,7 +1161,7 @@
         <v>28</v>
       </c>
       <c r="G3">
-        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$102,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$200,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>7</v>
       </c>
     </row>
@@ -1185,7 +1182,7 @@
         <v>31</v>
       </c>
       <c r="G4">
-        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$102,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$200,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>8</v>
       </c>
     </row>
@@ -1206,7 +1203,7 @@
         <v>33</v>
       </c>
       <c r="G5">
-        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$102,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$200,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>9</v>
       </c>
     </row>
@@ -1227,7 +1224,7 @@
         <v>36</v>
       </c>
       <c r="G6">
-        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$102,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$200,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>10</v>
       </c>
     </row>
@@ -1248,7 +1245,7 @@
         <v>39</v>
       </c>
       <c r="G7">
-        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$102,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$200,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>11</v>
       </c>
     </row>
@@ -1272,7 +1269,7 @@
         <v>175</v>
       </c>
       <c r="G8">
-        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$102,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$200,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>12</v>
       </c>
     </row>
@@ -1293,7 +1290,7 @@
         <v>44</v>
       </c>
       <c r="G9">
-        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$102,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$200,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>13</v>
       </c>
     </row>
@@ -1314,7 +1311,7 @@
         <v>232</v>
       </c>
       <c r="G10">
-        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$102,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$200,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>98</v>
       </c>
     </row>
@@ -1334,9 +1331,9 @@
       <c r="E11" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G11" t="e">
-        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$102,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>#N/A</v>
+      <c r="G11">
+        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$200,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1359,7 +1356,7 @@
         <v>42</v>
       </c>
       <c r="G12">
-        <f t="array" ref="G12">INDEX('All Checks'!$A$1:$G$102,MATCH(A12&amp;B12&amp;C12,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G12">INDEX('All Checks'!$A$1:$G$200,MATCH(A12&amp;B12&amp;C12,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>47</v>
       </c>
     </row>
@@ -1380,7 +1377,7 @@
         <v>44</v>
       </c>
       <c r="G13">
-        <f t="array" ref="G13">INDEX('All Checks'!$A$1:$G$102,MATCH(A13&amp;B13&amp;C13,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G13">INDEX('All Checks'!$A$1:$G$200,MATCH(A13&amp;B13&amp;C13,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>48</v>
       </c>
     </row>
@@ -1401,7 +1398,7 @@
         <v>185</v>
       </c>
       <c r="G14">
-        <f t="array" ref="G14">INDEX('All Checks'!$A$1:$G$102,MATCH(A14&amp;B14&amp;C14,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G14">INDEX('All Checks'!$A$1:$G$200,MATCH(A14&amp;B14&amp;C14,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>49</v>
       </c>
     </row>
@@ -1422,7 +1419,7 @@
         <v>186</v>
       </c>
       <c r="G15">
-        <f t="array" ref="G15">INDEX('All Checks'!$A$1:$G$102,MATCH(A15&amp;B15&amp;C15,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G15">INDEX('All Checks'!$A$1:$G$200,MATCH(A15&amp;B15&amp;C15,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>50</v>
       </c>
     </row>
@@ -1443,7 +1440,7 @@
         <v>187</v>
       </c>
       <c r="G16">
-        <f t="array" ref="G16">INDEX('All Checks'!$A$1:$G$102,MATCH(A16&amp;B16&amp;C16,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G16">INDEX('All Checks'!$A$1:$G$200,MATCH(A16&amp;B16&amp;C16,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>51</v>
       </c>
     </row>
@@ -1464,7 +1461,7 @@
         <v>188</v>
       </c>
       <c r="G17">
-        <f t="array" ref="G17">INDEX('All Checks'!$A$1:$G$102,MATCH(A17&amp;B17&amp;C17,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G17">INDEX('All Checks'!$A$1:$G$200,MATCH(A17&amp;B17&amp;C17,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>52</v>
       </c>
     </row>
@@ -1485,7 +1482,7 @@
         <v>189</v>
       </c>
       <c r="G18">
-        <f t="array" ref="G18">INDEX('All Checks'!$A$1:$G$102,MATCH(A18&amp;B18&amp;C18,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G18">INDEX('All Checks'!$A$1:$G$200,MATCH(A18&amp;B18&amp;C18,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>53</v>
       </c>
     </row>
@@ -1506,7 +1503,7 @@
         <v>190</v>
       </c>
       <c r="G19">
-        <f t="array" ref="G19">INDEX('All Checks'!$A$1:$G$102,MATCH(A19&amp;B19&amp;C19,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G19">INDEX('All Checks'!$A$1:$G$200,MATCH(A19&amp;B19&amp;C19,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>54</v>
       </c>
     </row>
@@ -1527,7 +1524,7 @@
         <v>192</v>
       </c>
       <c r="G20">
-        <f t="array" ref="G20">INDEX('All Checks'!$A$1:$G$102,MATCH(A20&amp;B20&amp;C20,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G20">INDEX('All Checks'!$A$1:$G$200,MATCH(A20&amp;B20&amp;C20,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>55</v>
       </c>
     </row>
@@ -1551,7 +1548,7 @@
         <v>145</v>
       </c>
       <c r="G21">
-        <f t="array" ref="G21">INDEX('All Checks'!$A$1:$G$102,MATCH(A21&amp;B21&amp;C21,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G21">INDEX('All Checks'!$A$1:$G$200,MATCH(A21&amp;B21&amp;C21,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>82</v>
       </c>
     </row>
@@ -1619,7 +1616,7 @@
         <v>22</v>
       </c>
       <c r="G2">
-        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$102,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$200,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>5</v>
       </c>
     </row>
@@ -1641,7 +1638,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3">
-        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$102,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$200,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>42</v>
       </c>
     </row>
@@ -1662,7 +1659,7 @@
         <v>103</v>
       </c>
       <c r="G4">
-        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$102,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$200,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>43</v>
       </c>
     </row>
@@ -1683,7 +1680,7 @@
         <v>106</v>
       </c>
       <c r="G5">
-        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$102,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$200,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>44</v>
       </c>
     </row>
@@ -1704,7 +1701,7 @@
         <v>109</v>
       </c>
       <c r="G6">
-        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$102,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$200,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>45</v>
       </c>
     </row>
@@ -1725,7 +1722,7 @@
         <v>111</v>
       </c>
       <c r="G7">
-        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$102,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$200,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>46</v>
       </c>
     </row>
@@ -1746,7 +1743,7 @@
         <v>215</v>
       </c>
       <c r="G8">
-        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$102,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$200,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>79</v>
       </c>
     </row>
@@ -1767,7 +1764,7 @@
         <v>218</v>
       </c>
       <c r="G9">
-        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$102,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$200,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>80</v>
       </c>
     </row>
@@ -1788,7 +1785,7 @@
         <v>144</v>
       </c>
       <c r="G10">
-        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$102,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$200,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>81</v>
       </c>
     </row>
@@ -1809,7 +1806,7 @@
         <v>148</v>
       </c>
       <c r="G11">
-        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$102,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$200,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>83</v>
       </c>
     </row>
@@ -1825,8 +1822,8 @@
   </sheetPr>
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1874,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$102,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$200,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>1</v>
       </c>
     </row>
@@ -1895,7 +1892,7 @@
         <v>13</v>
       </c>
       <c r="G3">
-        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$102,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$200,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>2</v>
       </c>
     </row>
@@ -1916,7 +1913,7 @@
         <v>15</v>
       </c>
       <c r="G4">
-        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$102,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$200,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>3</v>
       </c>
     </row>
@@ -1937,7 +1934,7 @@
         <v>17</v>
       </c>
       <c r="G5">
-        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$102,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$200,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>4</v>
       </c>
     </row>
@@ -1958,7 +1955,7 @@
         <v>176</v>
       </c>
       <c r="G6">
-        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$102,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$200,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>14</v>
       </c>
     </row>
@@ -1979,7 +1976,7 @@
         <v>155</v>
       </c>
       <c r="G7">
-        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$102,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$200,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>15</v>
       </c>
     </row>
@@ -2000,7 +1997,7 @@
         <v>50</v>
       </c>
       <c r="G8">
-        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$102,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$200,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>16</v>
       </c>
     </row>
@@ -2021,7 +2018,7 @@
         <v>155</v>
       </c>
       <c r="G9">
-        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$102,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$200,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>17</v>
       </c>
     </row>
@@ -2042,7 +2039,7 @@
         <v>53</v>
       </c>
       <c r="G10">
-        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$102,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$200,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>18</v>
       </c>
     </row>
@@ -2063,7 +2060,7 @@
         <v>155</v>
       </c>
       <c r="G11">
-        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$102,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$200,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>19</v>
       </c>
     </row>
@@ -2084,7 +2081,7 @@
         <v>155</v>
       </c>
       <c r="G12">
-        <f t="array" ref="G12">INDEX('All Checks'!$A$1:$G$102,MATCH(A12&amp;B12&amp;C12,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G12">INDEX('All Checks'!$A$1:$G$200,MATCH(A12&amp;B12&amp;C12,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>20</v>
       </c>
     </row>
@@ -2105,7 +2102,7 @@
         <v>155</v>
       </c>
       <c r="G13">
-        <f t="array" ref="G13">INDEX('All Checks'!$A$1:$G$102,MATCH(A13&amp;B13&amp;C13,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G13">INDEX('All Checks'!$A$1:$G$200,MATCH(A13&amp;B13&amp;C13,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>21</v>
       </c>
     </row>
@@ -2126,7 +2123,7 @@
         <v>155</v>
       </c>
       <c r="G14">
-        <f t="array" ref="G14">INDEX('All Checks'!$A$1:$G$102,MATCH(A14&amp;B14&amp;C14,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G14">INDEX('All Checks'!$A$1:$G$200,MATCH(A14&amp;B14&amp;C14,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>22</v>
       </c>
     </row>
@@ -2147,7 +2144,7 @@
         <v>155</v>
       </c>
       <c r="G15">
-        <f t="array" ref="G15">INDEX('All Checks'!$A$1:$G$102,MATCH(A15&amp;B15&amp;C15,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G15">INDEX('All Checks'!$A$1:$G$200,MATCH(A15&amp;B15&amp;C15,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>23</v>
       </c>
     </row>
@@ -2168,7 +2165,7 @@
         <v>155</v>
       </c>
       <c r="G16">
-        <f t="array" ref="G16">INDEX('All Checks'!$A$1:$G$102,MATCH(A16&amp;B16&amp;C16,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G16">INDEX('All Checks'!$A$1:$G$200,MATCH(A16&amp;B16&amp;C16,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>24</v>
       </c>
     </row>
@@ -2189,7 +2186,7 @@
         <v>155</v>
       </c>
       <c r="G17">
-        <f t="array" ref="G17">INDEX('All Checks'!$A$1:$G$102,MATCH(A17&amp;B17&amp;C17,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G17">INDEX('All Checks'!$A$1:$G$200,MATCH(A17&amp;B17&amp;C17,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>25</v>
       </c>
     </row>
@@ -2210,7 +2207,7 @@
         <v>155</v>
       </c>
       <c r="G18">
-        <f t="array" ref="G18">INDEX('All Checks'!$A$1:$G$102,MATCH(A18&amp;B18&amp;C18,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G18">INDEX('All Checks'!$A$1:$G$200,MATCH(A18&amp;B18&amp;C18,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>26</v>
       </c>
     </row>
@@ -2231,7 +2228,7 @@
         <v>155</v>
       </c>
       <c r="G19">
-        <f t="array" ref="G19">INDEX('All Checks'!$A$1:$G$102,MATCH(A19&amp;B19&amp;C19,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G19">INDEX('All Checks'!$A$1:$G$200,MATCH(A19&amp;B19&amp;C19,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>27</v>
       </c>
     </row>
@@ -2252,7 +2249,7 @@
         <v>155</v>
       </c>
       <c r="G20">
-        <f t="array" ref="G20">INDEX('All Checks'!$A$1:$G$102,MATCH(A20&amp;B20&amp;C20,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G20">INDEX('All Checks'!$A$1:$G$200,MATCH(A20&amp;B20&amp;C20,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>28</v>
       </c>
     </row>
@@ -2273,7 +2270,7 @@
         <v>155</v>
       </c>
       <c r="G21">
-        <f t="array" ref="G21">INDEX('All Checks'!$A$1:$G$102,MATCH(A21&amp;B21&amp;C21,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G21">INDEX('All Checks'!$A$1:$G$200,MATCH(A21&amp;B21&amp;C21,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>29</v>
       </c>
     </row>
@@ -2294,7 +2291,7 @@
         <v>155</v>
       </c>
       <c r="G22">
-        <f t="array" ref="G22">INDEX('All Checks'!$A$1:$G$102,MATCH(A22&amp;B22&amp;C22,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G22">INDEX('All Checks'!$A$1:$G$200,MATCH(A22&amp;B22&amp;C22,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>30</v>
       </c>
     </row>
@@ -2315,7 +2312,7 @@
         <v>155</v>
       </c>
       <c r="G23">
-        <f t="array" ref="G23">INDEX('All Checks'!$A$1:$G$102,MATCH(A23&amp;B23&amp;C23,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G23">INDEX('All Checks'!$A$1:$G$200,MATCH(A23&amp;B23&amp;C23,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>31</v>
       </c>
     </row>
@@ -2336,7 +2333,7 @@
         <v>155</v>
       </c>
       <c r="G24">
-        <f t="array" ref="G24">INDEX('All Checks'!$A$1:$G$102,MATCH(A24&amp;B24&amp;C24,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G24">INDEX('All Checks'!$A$1:$G$200,MATCH(A24&amp;B24&amp;C24,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>32</v>
       </c>
     </row>
@@ -2357,7 +2354,7 @@
         <v>182</v>
       </c>
       <c r="G25">
-        <f t="array" ref="G25">INDEX('All Checks'!$A$1:$G$102,MATCH(A25&amp;B25&amp;C25,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G25">INDEX('All Checks'!$A$1:$G$200,MATCH(A25&amp;B25&amp;C25,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>33</v>
       </c>
     </row>
@@ -2378,7 +2375,7 @@
         <v>183</v>
       </c>
       <c r="G26">
-        <f t="array" ref="G26">INDEX('All Checks'!$A$1:$G$102,MATCH(A26&amp;B26&amp;C26,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G26">INDEX('All Checks'!$A$1:$G$200,MATCH(A26&amp;B26&amp;C26,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>34</v>
       </c>
     </row>
@@ -2399,7 +2396,7 @@
         <v>183</v>
       </c>
       <c r="G27">
-        <f t="array" ref="G27">INDEX('All Checks'!$A$1:$G$102,MATCH(A27&amp;B27&amp;C27,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G27">INDEX('All Checks'!$A$1:$G$200,MATCH(A27&amp;B27&amp;C27,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>35</v>
       </c>
     </row>
@@ -2420,7 +2417,7 @@
         <v>155</v>
       </c>
       <c r="G28">
-        <f t="array" ref="G28">INDEX('All Checks'!$A$1:$G$102,MATCH(A28&amp;B28&amp;C28,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G28">INDEX('All Checks'!$A$1:$G$200,MATCH(A28&amp;B28&amp;C28,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>36</v>
       </c>
     </row>
@@ -2441,7 +2438,7 @@
         <v>155</v>
       </c>
       <c r="G29">
-        <f t="array" ref="G29">INDEX('All Checks'!$A$1:$G$102,MATCH(A29&amp;B29&amp;C29,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G29">INDEX('All Checks'!$A$1:$G$200,MATCH(A29&amp;B29&amp;C29,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>37</v>
       </c>
     </row>
@@ -2462,7 +2459,7 @@
         <v>155</v>
       </c>
       <c r="G30">
-        <f t="array" ref="G30">INDEX('All Checks'!$A$1:$G$102,MATCH(A30&amp;B30&amp;C30,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G30">INDEX('All Checks'!$A$1:$G$200,MATCH(A30&amp;B30&amp;C30,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>38</v>
       </c>
     </row>
@@ -2483,7 +2480,7 @@
         <v>182</v>
       </c>
       <c r="G31">
-        <f t="array" ref="G31">INDEX('All Checks'!$A$1:$G$102,MATCH(A31&amp;B31&amp;C31,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G31">INDEX('All Checks'!$A$1:$G$200,MATCH(A31&amp;B31&amp;C31,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>39</v>
       </c>
     </row>
@@ -2504,7 +2501,7 @@
         <v>95</v>
       </c>
       <c r="G32">
-        <f t="array" ref="G32">INDEX('All Checks'!$A$1:$G$102,MATCH(A32&amp;B32&amp;C32,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G32">INDEX('All Checks'!$A$1:$G$200,MATCH(A32&amp;B32&amp;C32,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>40</v>
       </c>
     </row>
@@ -2525,7 +2522,7 @@
         <v>98</v>
       </c>
       <c r="G33">
-        <f t="array" ref="G33">INDEX('All Checks'!$A$1:$G$102,MATCH(A33&amp;B33&amp;C33,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G33">INDEX('All Checks'!$A$1:$G$200,MATCH(A33&amp;B33&amp;C33,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>41</v>
       </c>
     </row>
@@ -2546,7 +2543,7 @@
         <v>123</v>
       </c>
       <c r="G34">
-        <f t="array" ref="G34">INDEX('All Checks'!$A$1:$G$102,MATCH(A34&amp;B34&amp;C34,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G34">INDEX('All Checks'!$A$1:$G$200,MATCH(A34&amp;B34&amp;C34,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>56</v>
       </c>
     </row>
@@ -2567,7 +2564,7 @@
         <v>123</v>
       </c>
       <c r="G35">
-        <f t="array" ref="G35">INDEX('All Checks'!$A$1:$G$102,MATCH(A35&amp;B35&amp;C35,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G35">INDEX('All Checks'!$A$1:$G$200,MATCH(A35&amp;B35&amp;C35,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>57</v>
       </c>
     </row>
@@ -2588,7 +2585,7 @@
         <v>123</v>
       </c>
       <c r="G36">
-        <f t="array" ref="G36">INDEX('All Checks'!$A$1:$G$102,MATCH(A36&amp;B36&amp;C36,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G36">INDEX('All Checks'!$A$1:$G$200,MATCH(A36&amp;B36&amp;C36,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>58</v>
       </c>
     </row>
@@ -2609,7 +2606,7 @@
         <v>123</v>
       </c>
       <c r="G37">
-        <f t="array" ref="G37">INDEX('All Checks'!$A$1:$G$102,MATCH(A37&amp;B37&amp;C37,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G37">INDEX('All Checks'!$A$1:$G$200,MATCH(A37&amp;B37&amp;C37,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>59</v>
       </c>
     </row>
@@ -2630,7 +2627,7 @@
         <v>123</v>
       </c>
       <c r="G38">
-        <f t="array" ref="G38">INDEX('All Checks'!$A$1:$G$102,MATCH(A38&amp;B38&amp;C38,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G38">INDEX('All Checks'!$A$1:$G$200,MATCH(A38&amp;B38&amp;C38,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>60</v>
       </c>
     </row>
@@ -2651,7 +2648,7 @@
         <v>123</v>
       </c>
       <c r="G39">
-        <f t="array" ref="G39">INDEX('All Checks'!$A$1:$G$102,MATCH(A39&amp;B39&amp;C39,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G39">INDEX('All Checks'!$A$1:$G$200,MATCH(A39&amp;B39&amp;C39,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>61</v>
       </c>
     </row>
@@ -2672,7 +2669,7 @@
         <v>123</v>
       </c>
       <c r="G40">
-        <f t="array" ref="G40">INDEX('All Checks'!$A$1:$G$102,MATCH(A40&amp;B40&amp;C40,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G40">INDEX('All Checks'!$A$1:$G$200,MATCH(A40&amp;B40&amp;C40,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>62</v>
       </c>
     </row>
@@ -2693,7 +2690,7 @@
         <v>123</v>
       </c>
       <c r="G41">
-        <f t="array" ref="G41">INDEX('All Checks'!$A$1:$G$102,MATCH(A41&amp;B41&amp;C41,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G41">INDEX('All Checks'!$A$1:$G$200,MATCH(A41&amp;B41&amp;C41,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>63</v>
       </c>
     </row>
@@ -2714,7 +2711,7 @@
         <v>123</v>
       </c>
       <c r="G42">
-        <f t="array" ref="G42">INDEX('All Checks'!$A$1:$G$102,MATCH(A42&amp;B42&amp;C42,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G42">INDEX('All Checks'!$A$1:$G$200,MATCH(A42&amp;B42&amp;C42,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>64</v>
       </c>
     </row>
@@ -2735,7 +2732,7 @@
         <v>123</v>
       </c>
       <c r="G43">
-        <f t="array" ref="G43">INDEX('All Checks'!$A$1:$G$102,MATCH(A43&amp;B43&amp;C43,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G43">INDEX('All Checks'!$A$1:$G$200,MATCH(A43&amp;B43&amp;C43,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>65</v>
       </c>
     </row>
@@ -2756,7 +2753,7 @@
         <v>123</v>
       </c>
       <c r="G44">
-        <f t="array" ref="G44">INDEX('All Checks'!$A$1:$G$102,MATCH(A44&amp;B44&amp;C44,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G44">INDEX('All Checks'!$A$1:$G$200,MATCH(A44&amp;B44&amp;C44,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>66</v>
       </c>
     </row>
@@ -2777,7 +2774,7 @@
         <v>123</v>
       </c>
       <c r="G45">
-        <f t="array" ref="G45">INDEX('All Checks'!$A$1:$G$102,MATCH(A45&amp;B45&amp;C45,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G45">INDEX('All Checks'!$A$1:$G$200,MATCH(A45&amp;B45&amp;C45,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>67</v>
       </c>
     </row>
@@ -2798,7 +2795,7 @@
         <v>123</v>
       </c>
       <c r="G46">
-        <f t="array" ref="G46">INDEX('All Checks'!$A$1:$G$102,MATCH(A46&amp;B46&amp;C46,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G46">INDEX('All Checks'!$A$1:$G$200,MATCH(A46&amp;B46&amp;C46,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>68</v>
       </c>
     </row>
@@ -2819,7 +2816,7 @@
         <v>206</v>
       </c>
       <c r="G47">
-        <f t="array" ref="G47">INDEX('All Checks'!$A$1:$G$102,MATCH(A47&amp;B47&amp;C47,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G47">INDEX('All Checks'!$A$1:$G$200,MATCH(A47&amp;B47&amp;C47,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>69</v>
       </c>
     </row>
@@ -2840,7 +2837,7 @@
         <v>208</v>
       </c>
       <c r="G48">
-        <f t="array" ref="G48">INDEX('All Checks'!$A$1:$G$102,MATCH(A48&amp;B48&amp;C48,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G48">INDEX('All Checks'!$A$1:$G$200,MATCH(A48&amp;B48&amp;C48,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>70</v>
       </c>
     </row>
@@ -2861,7 +2858,7 @@
         <v>209</v>
       </c>
       <c r="G49">
-        <f t="array" ref="G49">INDEX('All Checks'!$A$1:$G$102,MATCH(A49&amp;B49&amp;C49,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G49">INDEX('All Checks'!$A$1:$G$200,MATCH(A49&amp;B49&amp;C49,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>71</v>
       </c>
     </row>
@@ -2885,7 +2882,7 @@
         <v>132</v>
       </c>
       <c r="G50">
-        <f t="array" ref="G50">INDEX('All Checks'!$A$1:$G$102,MATCH(A50&amp;B50&amp;C50,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G50">INDEX('All Checks'!$A$1:$G$200,MATCH(A50&amp;B50&amp;C50,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>72</v>
       </c>
     </row>
@@ -2909,7 +2906,7 @@
         <v>132</v>
       </c>
       <c r="G51">
-        <f t="array" ref="G51">INDEX('All Checks'!$A$1:$G$102,MATCH(A51&amp;B51&amp;C51,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G51">INDEX('All Checks'!$A$1:$G$200,MATCH(A51&amp;B51&amp;C51,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>73</v>
       </c>
     </row>
@@ -2930,7 +2927,7 @@
         <v>123</v>
       </c>
       <c r="G52">
-        <f t="array" ref="G52">INDEX('All Checks'!$A$1:$G$102,MATCH(A52&amp;B52&amp;C52,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G52">INDEX('All Checks'!$A$1:$G$200,MATCH(A52&amp;B52&amp;C52,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>74</v>
       </c>
     </row>
@@ -2951,7 +2948,7 @@
         <v>138</v>
       </c>
       <c r="G53">
-        <f t="array" ref="G53">INDEX('All Checks'!$A$1:$G$102,MATCH(A53&amp;B53&amp;C53,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G53">INDEX('All Checks'!$A$1:$G$200,MATCH(A53&amp;B53&amp;C53,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>75</v>
       </c>
     </row>
@@ -2972,7 +2969,7 @@
         <v>211</v>
       </c>
       <c r="G54">
-        <f t="array" ref="G54">INDEX('All Checks'!$A$1:$G$102,MATCH(A54&amp;B54&amp;C54,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G54">INDEX('All Checks'!$A$1:$G$200,MATCH(A54&amp;B54&amp;C54,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>76</v>
       </c>
     </row>
@@ -2993,7 +2990,7 @@
         <v>212</v>
       </c>
       <c r="G55">
-        <f t="array" ref="G55">INDEX('All Checks'!$A$1:$G$102,MATCH(A55&amp;B55&amp;C55,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G55">INDEX('All Checks'!$A$1:$G$200,MATCH(A55&amp;B55&amp;C55,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>77</v>
       </c>
     </row>
@@ -3014,7 +3011,7 @@
         <v>123</v>
       </c>
       <c r="G56">
-        <f t="array" ref="G56">INDEX('All Checks'!$A$1:$G$102,MATCH(A56&amp;B56&amp;C56,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G56">INDEX('All Checks'!$A$1:$G$200,MATCH(A56&amp;B56&amp;C56,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>78</v>
       </c>
     </row>
@@ -3035,7 +3032,7 @@
         <v>150</v>
       </c>
       <c r="G57">
-        <f t="array" ref="G57">INDEX('All Checks'!$A$1:$G$102,MATCH(A57&amp;B57&amp;C57,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G57">INDEX('All Checks'!$A$1:$G$200,MATCH(A57&amp;B57&amp;C57,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>84</v>
       </c>
     </row>
@@ -3056,7 +3053,7 @@
         <v>221</v>
       </c>
       <c r="G58">
-        <f t="array" ref="G58">INDEX('All Checks'!$A$1:$G$102,MATCH(A58&amp;B58&amp;C58,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G58">INDEX('All Checks'!$A$1:$G$200,MATCH(A58&amp;B58&amp;C58,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>85</v>
       </c>
     </row>
@@ -3077,7 +3074,7 @@
         <v>153</v>
       </c>
       <c r="G59">
-        <f t="array" ref="G59">INDEX('All Checks'!$A$1:$G$102,MATCH(A59&amp;B59&amp;C59,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G59">INDEX('All Checks'!$A$1:$G$200,MATCH(A59&amp;B59&amp;C59,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>86</v>
       </c>
     </row>
@@ -3098,7 +3095,7 @@
         <v>155</v>
       </c>
       <c r="G60">
-        <f t="array" ref="G60">INDEX('All Checks'!$A$1:$G$102,MATCH(A60&amp;B60&amp;C60,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G60">INDEX('All Checks'!$A$1:$G$200,MATCH(A60&amp;B60&amp;C60,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>87</v>
       </c>
     </row>
@@ -3119,7 +3116,7 @@
         <v>157</v>
       </c>
       <c r="G61">
-        <f t="array" ref="G61">INDEX('All Checks'!$A$1:$G$102,MATCH(A61&amp;B61&amp;C61,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G61">INDEX('All Checks'!$A$1:$G$200,MATCH(A61&amp;B61&amp;C61,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>88</v>
       </c>
     </row>
@@ -3140,7 +3137,7 @@
         <v>159</v>
       </c>
       <c r="G62">
-        <f t="array" ref="G62">INDEX('All Checks'!$A$1:$G$102,MATCH(A62&amp;B62&amp;C62,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G62">INDEX('All Checks'!$A$1:$G$200,MATCH(A62&amp;B62&amp;C62,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>89</v>
       </c>
     </row>
@@ -3161,7 +3158,7 @@
         <v>157</v>
       </c>
       <c r="G63">
-        <f t="array" ref="G63">INDEX('All Checks'!$A$1:$G$102,MATCH(A63&amp;B63&amp;C63,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G63">INDEX('All Checks'!$A$1:$G$200,MATCH(A63&amp;B63&amp;C63,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>90</v>
       </c>
     </row>
@@ -3182,7 +3179,7 @@
         <v>225</v>
       </c>
       <c r="G64">
-        <f t="array" ref="G64">INDEX('All Checks'!$A$1:$G$102,MATCH(A64&amp;B64&amp;C64,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G64">INDEX('All Checks'!$A$1:$G$200,MATCH(A64&amp;B64&amp;C64,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>91</v>
       </c>
     </row>
@@ -3203,7 +3200,7 @@
         <v>155</v>
       </c>
       <c r="G65">
-        <f t="array" ref="G65">INDEX('All Checks'!$A$1:$G$102,MATCH(A65&amp;B65&amp;C65,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G65">INDEX('All Checks'!$A$1:$G$200,MATCH(A65&amp;B65&amp;C65,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>92</v>
       </c>
     </row>
@@ -3224,7 +3221,7 @@
         <v>159</v>
       </c>
       <c r="G66">
-        <f t="array" ref="G66">INDEX('All Checks'!$A$1:$G$102,MATCH(A66&amp;B66&amp;C66,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G66">INDEX('All Checks'!$A$1:$G$200,MATCH(A66&amp;B66&amp;C66,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>93</v>
       </c>
     </row>
@@ -3245,7 +3242,7 @@
         <v>227</v>
       </c>
       <c r="G67">
-        <f t="array" ref="G67">INDEX('All Checks'!$A$1:$G$102,MATCH(A67&amp;B67&amp;C67,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G67">INDEX('All Checks'!$A$1:$G$200,MATCH(A67&amp;B67&amp;C67,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>94</v>
       </c>
     </row>
@@ -3266,7 +3263,7 @@
         <v>228</v>
       </c>
       <c r="G68">
-        <f t="array" ref="G68">INDEX('All Checks'!$A$1:$G$102,MATCH(A68&amp;B68&amp;C68,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G68">INDEX('All Checks'!$A$1:$G$200,MATCH(A68&amp;B68&amp;C68,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>95</v>
       </c>
     </row>
@@ -3287,7 +3284,7 @@
         <v>155</v>
       </c>
       <c r="G69">
-        <f t="array" ref="G69">INDEX('All Checks'!$A$1:$G$102,MATCH(A69&amp;B69&amp;C69,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G69">INDEX('All Checks'!$A$1:$G$200,MATCH(A69&amp;B69&amp;C69,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>96</v>
       </c>
     </row>
@@ -3308,7 +3305,7 @@
         <v>230</v>
       </c>
       <c r="G70">
-        <f t="array" ref="G70">INDEX('All Checks'!$A$1:$G$102,MATCH(A70&amp;B70&amp;C70,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G70">INDEX('All Checks'!$A$1:$G$200,MATCH(A70&amp;B70&amp;C70,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>97</v>
       </c>
     </row>
@@ -3329,7 +3326,7 @@
         <v>234</v>
       </c>
       <c r="G71">
-        <f t="array" ref="G71">INDEX('All Checks'!$A$1:$G$102,MATCH(A71&amp;B71&amp;C71,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G71">INDEX('All Checks'!$A$1:$G$200,MATCH(A71&amp;B71&amp;C71,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>99</v>
       </c>
     </row>
@@ -3350,7 +3347,7 @@
         <v>171</v>
       </c>
       <c r="G72">
-        <f t="array" ref="G72">INDEX('All Checks'!$A$1:$G$102,MATCH(A72&amp;B72&amp;C72,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <f t="array" ref="G72">INDEX('All Checks'!$A$1:$G$200,MATCH(A72&amp;B72&amp;C72,'All Checks'!$A$1:$A$200&amp;'All Checks'!$B$1:$B$200&amp;'All Checks'!$C$1:$C$200,0),7)</f>
         <v>100</v>
       </c>
     </row>
@@ -3366,8 +3363,8 @@
   </sheetPr>
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4872,7 +4869,7 @@
         <v>127</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>238</v>
+        <v>126</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>208</v>
@@ -5498,22 +5495,21 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C101" s="1" t="s">
+      <c r="A101" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F101" s="1"/>
       <c r="G101">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
organized by source and type since we added new checks
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="8510" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="6410" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="File Structure" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="All Checks" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$104</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="245">
   <si>
     <t>Source</t>
   </si>
@@ -648,9 +648,6 @@
     <t>This client has an Approximate Date Homelessness Started in their enrollment that is after their Project Start Date. The information at Project Start should reflect the client's situation at the point of Project Start, so this date may have been incorrectly entered.</t>
   </si>
   <si>
-    <t>3.10 - Project Start Date, 3.917.3 - Prior Living Situation: Date</t>
-  </si>
-  <si>
     <t>According to this client's assessment at Project Start, they experienced a single episode of homelessness in the three years prior to their Project Start and the approximate date homelessness started is known, but there was no response entered for the total number of months they experienced homelessness prior to this enrollment. It should be possible to determine and enter the total number of months they experienced homelessness based on the Approximate Date Homelessness Started and the Project Start Date.</t>
   </si>
   <si>
@@ -754,6 +751,15 @@
   </si>
   <si>
     <t>This enrollment has been active without any updates to their Current Living Situation for longer than the days set for this Project Type in your Long Stayers settings on the Edit Local Settings tab. Please be sure that any CLS updates or project exits are reflected in HMIS.</t>
+  </si>
+  <si>
+    <t>Includes Services Only, Other, and Day Shelter</t>
+  </si>
+  <si>
+    <t>Includes ES-NbN, Street Outreach, and Coordinated Entry</t>
+  </si>
+  <si>
+    <t>4.12.1 - Information Date</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1108,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G21"/>
+      <selection activeCell="A2" sqref="A2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,7 +1138,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1155,7 +1161,6 @@
         <v>175</v>
       </c>
       <c r="G2">
-        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$102,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>6</v>
       </c>
     </row>
@@ -1176,7 +1181,6 @@
         <v>28</v>
       </c>
       <c r="G3">
-        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$102,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>7</v>
       </c>
     </row>
@@ -1197,7 +1201,6 @@
         <v>31</v>
       </c>
       <c r="G4">
-        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$102,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>8</v>
       </c>
     </row>
@@ -1218,7 +1221,6 @@
         <v>33</v>
       </c>
       <c r="G5">
-        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$102,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>9</v>
       </c>
     </row>
@@ -1239,7 +1241,6 @@
         <v>36</v>
       </c>
       <c r="G6">
-        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$102,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>10</v>
       </c>
     </row>
@@ -1260,7 +1261,6 @@
         <v>39</v>
       </c>
       <c r="G7">
-        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$102,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>11</v>
       </c>
     </row>
@@ -1284,7 +1284,6 @@
         <v>175</v>
       </c>
       <c r="G8">
-        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$102,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>12</v>
       </c>
     </row>
@@ -1304,8 +1303,10 @@
       <c r="E9" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="G9">
-        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$102,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>13</v>
       </c>
     </row>
@@ -1320,13 +1321,12 @@
         <v>168</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="G10">
-        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$102,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>98</v>
       </c>
     </row>
@@ -1341,14 +1341,13 @@
         <v>172</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G11" t="e">
-        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$102,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>#N/A</v>
+      <c r="G11">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1371,7 +1370,6 @@
         <v>42</v>
       </c>
       <c r="G12">
-        <f t="array" ref="G12">INDEX('All Checks'!$A$1:$G$102,MATCH(A12&amp;B12&amp;C12,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>47</v>
       </c>
     </row>
@@ -1392,7 +1390,6 @@
         <v>44</v>
       </c>
       <c r="G13">
-        <f t="array" ref="G13">INDEX('All Checks'!$A$1:$G$102,MATCH(A13&amp;B13&amp;C13,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>48</v>
       </c>
     </row>
@@ -1413,7 +1410,6 @@
         <v>185</v>
       </c>
       <c r="G14">
-        <f t="array" ref="G14">INDEX('All Checks'!$A$1:$G$102,MATCH(A14&amp;B14&amp;C14,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>49</v>
       </c>
     </row>
@@ -1434,7 +1430,6 @@
         <v>186</v>
       </c>
       <c r="G15">
-        <f t="array" ref="G15">INDEX('All Checks'!$A$1:$G$102,MATCH(A15&amp;B15&amp;C15,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>50</v>
       </c>
     </row>
@@ -1455,7 +1450,6 @@
         <v>187</v>
       </c>
       <c r="G16">
-        <f t="array" ref="G16">INDEX('All Checks'!$A$1:$G$102,MATCH(A16&amp;B16&amp;C16,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>51</v>
       </c>
     </row>
@@ -1476,7 +1470,6 @@
         <v>188</v>
       </c>
       <c r="G17">
-        <f t="array" ref="G17">INDEX('All Checks'!$A$1:$G$102,MATCH(A17&amp;B17&amp;C17,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>52</v>
       </c>
     </row>
@@ -1497,7 +1490,6 @@
         <v>189</v>
       </c>
       <c r="G18">
-        <f t="array" ref="G18">INDEX('All Checks'!$A$1:$G$102,MATCH(A18&amp;B18&amp;C18,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>53</v>
       </c>
     </row>
@@ -1518,7 +1510,6 @@
         <v>190</v>
       </c>
       <c r="G19">
-        <f t="array" ref="G19">INDEX('All Checks'!$A$1:$G$102,MATCH(A19&amp;B19&amp;C19,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>54</v>
       </c>
     </row>
@@ -1539,7 +1530,6 @@
         <v>192</v>
       </c>
       <c r="G20">
-        <f t="array" ref="G20">INDEX('All Checks'!$A$1:$G$102,MATCH(A20&amp;B20&amp;C20,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>55</v>
       </c>
     </row>
@@ -1563,7 +1553,6 @@
         <v>145</v>
       </c>
       <c r="G21">
-        <f t="array" ref="G21">INDEX('All Checks'!$A$1:$G$102,MATCH(A21&amp;B21&amp;C21,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>82</v>
       </c>
     </row>
@@ -1580,7 +1569,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G11"/>
+      <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1608,7 +1597,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1631,7 +1620,6 @@
         <v>22</v>
       </c>
       <c r="G2">
-        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$102,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>5</v>
       </c>
     </row>
@@ -1653,7 +1641,6 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3">
-        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$102,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>42</v>
       </c>
     </row>
@@ -1674,7 +1661,6 @@
         <v>103</v>
       </c>
       <c r="G4">
-        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$102,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>43</v>
       </c>
     </row>
@@ -1695,7 +1681,6 @@
         <v>106</v>
       </c>
       <c r="G5">
-        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$102,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>44</v>
       </c>
     </row>
@@ -1716,7 +1701,6 @@
         <v>109</v>
       </c>
       <c r="G6">
-        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$102,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>45</v>
       </c>
     </row>
@@ -1737,7 +1721,6 @@
         <v>111</v>
       </c>
       <c r="G7">
-        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$102,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>46</v>
       </c>
     </row>
@@ -1749,16 +1732,15 @@
         <v>122</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G8">
-        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$102,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>79</v>
       </c>
     </row>
@@ -1770,16 +1752,15 @@
         <v>122</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="G9">
-        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$102,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>80</v>
       </c>
     </row>
@@ -1800,7 +1781,6 @@
         <v>144</v>
       </c>
       <c r="G10">
-        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$102,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>81</v>
       </c>
     </row>
@@ -1821,7 +1801,6 @@
         <v>148</v>
       </c>
       <c r="G11">
-        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$102,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>83</v>
       </c>
     </row>
@@ -1835,10 +1814,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1866,7 +1845,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1886,7 +1865,6 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <f t="array" ref="G2">INDEX('All Checks'!$A$1:$G$102,MATCH(A2&amp;B2&amp;C2,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>1</v>
       </c>
     </row>
@@ -1907,7 +1885,6 @@
         <v>13</v>
       </c>
       <c r="G3">
-        <f t="array" ref="G3">INDEX('All Checks'!$A$1:$G$102,MATCH(A3&amp;B3&amp;C3,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>2</v>
       </c>
     </row>
@@ -1928,7 +1905,6 @@
         <v>15</v>
       </c>
       <c r="G4">
-        <f t="array" ref="G4">INDEX('All Checks'!$A$1:$G$102,MATCH(A4&amp;B4&amp;C4,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>3</v>
       </c>
     </row>
@@ -1949,7 +1925,6 @@
         <v>17</v>
       </c>
       <c r="G5">
-        <f t="array" ref="G5">INDEX('All Checks'!$A$1:$G$102,MATCH(A5&amp;B5&amp;C5,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>4</v>
       </c>
     </row>
@@ -1970,7 +1945,6 @@
         <v>176</v>
       </c>
       <c r="G6">
-        <f t="array" ref="G6">INDEX('All Checks'!$A$1:$G$102,MATCH(A6&amp;B6&amp;C6,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>14</v>
       </c>
     </row>
@@ -1991,7 +1965,6 @@
         <v>155</v>
       </c>
       <c r="G7">
-        <f t="array" ref="G7">INDEX('All Checks'!$A$1:$G$102,MATCH(A7&amp;B7&amp;C7,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>15</v>
       </c>
     </row>
@@ -2012,7 +1985,6 @@
         <v>50</v>
       </c>
       <c r="G8">
-        <f t="array" ref="G8">INDEX('All Checks'!$A$1:$G$102,MATCH(A8&amp;B8&amp;C8,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>16</v>
       </c>
     </row>
@@ -2033,7 +2005,6 @@
         <v>155</v>
       </c>
       <c r="G9">
-        <f t="array" ref="G9">INDEX('All Checks'!$A$1:$G$102,MATCH(A9&amp;B9&amp;C9,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>17</v>
       </c>
     </row>
@@ -2054,7 +2025,6 @@
         <v>53</v>
       </c>
       <c r="G10">
-        <f t="array" ref="G10">INDEX('All Checks'!$A$1:$G$102,MATCH(A10&amp;B10&amp;C10,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>18</v>
       </c>
     </row>
@@ -2075,7 +2045,6 @@
         <v>155</v>
       </c>
       <c r="G11">
-        <f t="array" ref="G11">INDEX('All Checks'!$A$1:$G$102,MATCH(A11&amp;B11&amp;C11,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>19</v>
       </c>
     </row>
@@ -2096,7 +2065,6 @@
         <v>155</v>
       </c>
       <c r="G12">
-        <f t="array" ref="G12">INDEX('All Checks'!$A$1:$G$102,MATCH(A12&amp;B12&amp;C12,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>20</v>
       </c>
     </row>
@@ -2117,7 +2085,6 @@
         <v>155</v>
       </c>
       <c r="G13">
-        <f t="array" ref="G13">INDEX('All Checks'!$A$1:$G$102,MATCH(A13&amp;B13&amp;C13,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>21</v>
       </c>
     </row>
@@ -2138,7 +2105,6 @@
         <v>155</v>
       </c>
       <c r="G14">
-        <f t="array" ref="G14">INDEX('All Checks'!$A$1:$G$102,MATCH(A14&amp;B14&amp;C14,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>22</v>
       </c>
     </row>
@@ -2159,7 +2125,6 @@
         <v>155</v>
       </c>
       <c r="G15">
-        <f t="array" ref="G15">INDEX('All Checks'!$A$1:$G$102,MATCH(A15&amp;B15&amp;C15,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>23</v>
       </c>
     </row>
@@ -2180,7 +2145,6 @@
         <v>155</v>
       </c>
       <c r="G16">
-        <f t="array" ref="G16">INDEX('All Checks'!$A$1:$G$102,MATCH(A16&amp;B16&amp;C16,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>24</v>
       </c>
     </row>
@@ -2201,7 +2165,6 @@
         <v>155</v>
       </c>
       <c r="G17">
-        <f t="array" ref="G17">INDEX('All Checks'!$A$1:$G$102,MATCH(A17&amp;B17&amp;C17,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>25</v>
       </c>
     </row>
@@ -2222,7 +2185,6 @@
         <v>155</v>
       </c>
       <c r="G18">
-        <f t="array" ref="G18">INDEX('All Checks'!$A$1:$G$102,MATCH(A18&amp;B18&amp;C18,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>26</v>
       </c>
     </row>
@@ -2243,7 +2205,6 @@
         <v>155</v>
       </c>
       <c r="G19">
-        <f t="array" ref="G19">INDEX('All Checks'!$A$1:$G$102,MATCH(A19&amp;B19&amp;C19,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>27</v>
       </c>
     </row>
@@ -2264,7 +2225,6 @@
         <v>155</v>
       </c>
       <c r="G20">
-        <f t="array" ref="G20">INDEX('All Checks'!$A$1:$G$102,MATCH(A20&amp;B20&amp;C20,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>28</v>
       </c>
     </row>
@@ -2285,7 +2245,6 @@
         <v>155</v>
       </c>
       <c r="G21">
-        <f t="array" ref="G21">INDEX('All Checks'!$A$1:$G$102,MATCH(A21&amp;B21&amp;C21,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>29</v>
       </c>
     </row>
@@ -2306,7 +2265,6 @@
         <v>155</v>
       </c>
       <c r="G22">
-        <f t="array" ref="G22">INDEX('All Checks'!$A$1:$G$102,MATCH(A22&amp;B22&amp;C22,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>30</v>
       </c>
     </row>
@@ -2327,7 +2285,6 @@
         <v>155</v>
       </c>
       <c r="G23">
-        <f t="array" ref="G23">INDEX('All Checks'!$A$1:$G$102,MATCH(A23&amp;B23&amp;C23,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>31</v>
       </c>
     </row>
@@ -2348,7 +2305,6 @@
         <v>155</v>
       </c>
       <c r="G24">
-        <f t="array" ref="G24">INDEX('All Checks'!$A$1:$G$102,MATCH(A24&amp;B24&amp;C24,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>32</v>
       </c>
     </row>
@@ -2369,7 +2325,6 @@
         <v>182</v>
       </c>
       <c r="G25">
-        <f t="array" ref="G25">INDEX('All Checks'!$A$1:$G$102,MATCH(A25&amp;B25&amp;C25,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>33</v>
       </c>
     </row>
@@ -2390,7 +2345,6 @@
         <v>183</v>
       </c>
       <c r="G26">
-        <f t="array" ref="G26">INDEX('All Checks'!$A$1:$G$102,MATCH(A26&amp;B26&amp;C26,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>34</v>
       </c>
     </row>
@@ -2411,7 +2365,6 @@
         <v>183</v>
       </c>
       <c r="G27">
-        <f t="array" ref="G27">INDEX('All Checks'!$A$1:$G$102,MATCH(A27&amp;B27&amp;C27,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>35</v>
       </c>
     </row>
@@ -2432,7 +2385,6 @@
         <v>155</v>
       </c>
       <c r="G28">
-        <f t="array" ref="G28">INDEX('All Checks'!$A$1:$G$102,MATCH(A28&amp;B28&amp;C28,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>36</v>
       </c>
     </row>
@@ -2453,7 +2405,6 @@
         <v>155</v>
       </c>
       <c r="G29">
-        <f t="array" ref="G29">INDEX('All Checks'!$A$1:$G$102,MATCH(A29&amp;B29&amp;C29,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>37</v>
       </c>
     </row>
@@ -2474,7 +2425,6 @@
         <v>155</v>
       </c>
       <c r="G30">
-        <f t="array" ref="G30">INDEX('All Checks'!$A$1:$G$102,MATCH(A30&amp;B30&amp;C30,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>38</v>
       </c>
     </row>
@@ -2495,7 +2445,6 @@
         <v>182</v>
       </c>
       <c r="G31">
-        <f t="array" ref="G31">INDEX('All Checks'!$A$1:$G$102,MATCH(A31&amp;B31&amp;C31,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>39</v>
       </c>
     </row>
@@ -2516,7 +2465,6 @@
         <v>95</v>
       </c>
       <c r="G32">
-        <f t="array" ref="G32">INDEX('All Checks'!$A$1:$G$102,MATCH(A32&amp;B32&amp;C32,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>40</v>
       </c>
     </row>
@@ -2537,323 +2485,307 @@
         <v>98</v>
       </c>
       <c r="G33">
-        <f t="array" ref="G33">INDEX('All Checks'!$A$1:$G$102,MATCH(A33&amp;B33&amp;C33,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>181</v>
+        <v>218</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="G34">
-        <f t="array" ref="G34">INDEX('All Checks'!$A$1:$G$102,MATCH(A34&amp;B34&amp;C34,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>123</v>
+        <v>220</v>
       </c>
       <c r="G35">
-        <f t="array" ref="G35">INDEX('All Checks'!$A$1:$G$102,MATCH(A35&amp;B35&amp;C35,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="G36">
-        <f t="array" ref="G36">INDEX('All Checks'!$A$1:$G$102,MATCH(A36&amp;B36&amp;C36,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>120</v>
+        <v>222</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="G37">
-        <f t="array" ref="G37">INDEX('All Checks'!$A$1:$G$102,MATCH(A37&amp;B37&amp;C37,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>197</v>
+        <v>156</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>82</v>
+        <v>222</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="G38">
-        <f t="array" ref="G38">INDEX('All Checks'!$A$1:$G$102,MATCH(A38&amp;B38&amp;C38,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>76</v>
+        <v>222</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="G39">
-        <f t="array" ref="G39">INDEX('All Checks'!$A$1:$G$102,MATCH(A39&amp;B39&amp;C39,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>88</v>
+        <v>222</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="G40">
-        <f t="array" ref="G40">INDEX('All Checks'!$A$1:$G$102,MATCH(A40&amp;B40&amp;C40,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>86</v>
+        <v>223</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>123</v>
+        <v>224</v>
       </c>
       <c r="G41">
-        <f t="array" ref="G41">INDEX('All Checks'!$A$1:$G$102,MATCH(A41&amp;B41&amp;C41,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>74</v>
+        <v>225</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="G42">
-        <f t="array" ref="G42">INDEX('All Checks'!$A$1:$G$102,MATCH(A42&amp;B42&amp;C42,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="G43">
-        <f t="array" ref="G43">INDEX('All Checks'!$A$1:$G$102,MATCH(A43&amp;B43&amp;C43,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>92</v>
+        <v>225</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>123</v>
+        <v>226</v>
       </c>
       <c r="G44">
-        <f t="array" ref="G44">INDEX('All Checks'!$A$1:$G$102,MATCH(A44&amp;B44&amp;C44,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>124</v>
+        <v>225</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
       <c r="G45">
-        <f t="array" ref="G45">INDEX('All Checks'!$A$1:$G$102,MATCH(A45&amp;B45&amp;C45,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="D46" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G46">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G47">
         <v>97</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G46">
-        <f t="array" ref="G46">INDEX('All Checks'!$A$1:$G$102,MATCH(A46&amp;B46&amp;C46,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G47">
-        <f t="array" ref="G47">INDEX('All Checks'!$A$1:$G$102,MATCH(A47&amp;B47&amp;C47,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>127</v>
+        <v>169</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="G48">
-        <f t="array" ref="G48">INDEX('All Checks'!$A$1:$G$102,MATCH(A48&amp;B48&amp;C48,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2864,17 +2796,16 @@
         <v>122</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>128</v>
+        <v>193</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>209</v>
+        <v>123</v>
       </c>
       <c r="G49">
-        <f t="array" ref="G49">INDEX('All Checks'!$A$1:$G$102,MATCH(A49&amp;B49&amp;C49,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2885,20 +2816,16 @@
         <v>122</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>130</v>
+        <v>194</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G50">
-        <f t="array" ref="G50">INDEX('All Checks'!$A$1:$G$102,MATCH(A50&amp;B50&amp;C50,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2909,20 +2836,16 @@
         <v>122</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>47</v>
+        <v>180</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G51">
-        <f t="array" ref="G51">INDEX('All Checks'!$A$1:$G$102,MATCH(A51&amp;B51&amp;C51,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2933,7 +2856,7 @@
         <v>122</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>135</v>
+        <v>196</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>120</v>
@@ -2942,8 +2865,7 @@
         <v>123</v>
       </c>
       <c r="G52">
-        <f t="array" ref="G52">INDEX('All Checks'!$A$1:$G$102,MATCH(A52&amp;B52&amp;C52,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2954,17 +2876,16 @@
         <v>122</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="G53">
-        <f t="array" ref="G53">INDEX('All Checks'!$A$1:$G$102,MATCH(A53&amp;B53&amp;C53,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2975,17 +2896,16 @@
         <v>122</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>211</v>
+        <v>123</v>
       </c>
       <c r="G54">
-        <f t="array" ref="G54">INDEX('All Checks'!$A$1:$G$102,MATCH(A54&amp;B54&amp;C54,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2996,17 +2916,16 @@
         <v>122</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>212</v>
+        <v>123</v>
       </c>
       <c r="G55">
-        <f t="array" ref="G55">INDEX('All Checks'!$A$1:$G$102,MATCH(A55&amp;B55&amp;C55,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3017,332 +2936,322 @@
         <v>122</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>123</v>
       </c>
       <c r="G56">
-        <f t="array" ref="G56">INDEX('All Checks'!$A$1:$G$102,MATCH(A56&amp;B56&amp;C56,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G57">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G58">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G59">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G60">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G61">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G62">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G63">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G64">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G65">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G66">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G67">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G68">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G69">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G70">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G71">
         <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G57">
-        <f t="array" ref="G57">INDEX('All Checks'!$A$1:$G$102,MATCH(A57&amp;B57&amp;C57,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="G58">
-        <f t="array" ref="G58">INDEX('All Checks'!$A$1:$G$102,MATCH(A58&amp;B58&amp;C58,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G59">
-        <f t="array" ref="G59">INDEX('All Checks'!$A$1:$G$102,MATCH(A59&amp;B59&amp;C59,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G60">
-        <f t="array" ref="G60">INDEX('All Checks'!$A$1:$G$102,MATCH(A60&amp;B60&amp;C60,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G61">
-        <f t="array" ref="G61">INDEX('All Checks'!$A$1:$G$102,MATCH(A61&amp;B61&amp;C61,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G62">
-        <f t="array" ref="G62">INDEX('All Checks'!$A$1:$G$102,MATCH(A62&amp;B62&amp;C62,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G63">
-        <f t="array" ref="G63">INDEX('All Checks'!$A$1:$G$102,MATCH(A63&amp;B63&amp;C63,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G64">
-        <f t="array" ref="G64">INDEX('All Checks'!$A$1:$G$102,MATCH(A64&amp;B64&amp;C64,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G65">
-        <f t="array" ref="G65">INDEX('All Checks'!$A$1:$G$102,MATCH(A65&amp;B65&amp;C65,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G66">
-        <f t="array" ref="G66">INDEX('All Checks'!$A$1:$G$102,MATCH(A66&amp;B66&amp;C66,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G67">
-        <f t="array" ref="G67">INDEX('All Checks'!$A$1:$G$102,MATCH(A67&amp;B67&amp;C67,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="G68">
-        <f t="array" ref="G68">INDEX('All Checks'!$A$1:$G$102,MATCH(A68&amp;B68&amp;C68,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G69">
-        <f t="array" ref="G69">INDEX('All Checks'!$A$1:$G$102,MATCH(A69&amp;B69&amp;C69,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="G70">
-        <f t="array" ref="G70">INDEX('All Checks'!$A$1:$G$102,MATCH(A70&amp;B70&amp;C70,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="G71">
-        <f t="array" ref="G71">INDEX('All Checks'!$A$1:$G$102,MATCH(A71&amp;B71&amp;C71,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
-        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -3356,14 +3265,59 @@
         <v>170</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>171</v>
       </c>
       <c r="G72">
-        <f t="array" ref="G72">INDEX('All Checks'!$A$1:$G$102,MATCH(A72&amp;B72&amp;C72,'All Checks'!$A$1:$A$101&amp;'All Checks'!$B$1:$B$101&amp;'All Checks'!$C$1:$C$101,0),7)</f>
         <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G73">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G74">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3378,8 +3332,8 @@
   </sheetPr>
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3411,7 +3365,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3697,44 +3651,43 @@
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>168</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>230</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>176</v>
+        <v>231</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15">
-        <v>14</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F16" s="1"/>
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="G16">
-        <v>15</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3745,17 +3698,17 @@
         <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>177</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3766,17 +3719,17 @@
         <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3787,17 +3740,17 @@
         <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3808,17 +3761,17 @@
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3829,17 +3782,17 @@
         <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3850,17 +3803,17 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3871,17 +3824,17 @@
         <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>180</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3892,17 +3845,17 @@
         <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3913,17 +3866,17 @@
         <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3934,17 +3887,17 @@
         <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3955,17 +3908,17 @@
         <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3976,17 +3929,17 @@
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3997,17 +3950,17 @@
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4018,17 +3971,17 @@
         <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4039,17 +3992,17 @@
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4060,17 +4013,17 @@
         <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4081,17 +4034,17 @@
         <v>45</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4102,17 +4055,17 @@
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4123,17 +4076,17 @@
         <v>45</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4144,17 +4097,17 @@
         <v>45</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4165,17 +4118,17 @@
         <v>45</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4186,17 +4139,17 @@
         <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4207,17 +4160,17 @@
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4228,17 +4181,17 @@
         <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4249,17 +4202,17 @@
         <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4270,313 +4223,311 @@
         <v>45</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>98</v>
+        <v>182</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F43" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="F43" s="1"/>
       <c r="G43">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>105</v>
+        <v>218</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45">
-        <v>44</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>109</v>
+        <v>220</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46">
-        <v>45</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>110</v>
+        <v>221</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47">
-        <v>46</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
+        <v>222</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="F48" s="1"/>
       <c r="G48">
-        <v>47</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49">
-        <v>48</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>113</v>
+        <v>222</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50">
-        <v>49</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>115</v>
+        <v>222</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>80</v>
+        <v>223</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52">
-        <v>51</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>74</v>
+        <v>225</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53">
-        <v>52</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>12</v>
+        <v>225</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54">
-        <v>53</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>120</v>
+        <v>225</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55">
-        <v>54</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56">
-        <v>55</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4584,20 +4535,20 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>181</v>
+        <v>228</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4605,20 +4556,20 @@
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>123</v>
+        <v>229</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58">
-        <v>57</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4626,316 +4577,316 @@
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>180</v>
+        <v>232</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>123</v>
+        <v>233</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>196</v>
+        <v>99</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="F60" s="2"/>
       <c r="G60">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>197</v>
+        <v>101</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>198</v>
+        <v>104</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>201</v>
+        <v>37</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="G65">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>203</v>
+        <v>112</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>123</v>
+        <v>187</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>238</v>
+        <v>12</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="F73" s="1"/>
       <c r="G73">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4946,19 +4897,17 @@
         <v>122</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>133</v>
+        <v>193</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>47</v>
+        <v>181</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>132</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="F74" s="1"/>
       <c r="G74">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4969,17 +4918,17 @@
         <v>122</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>123</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4990,17 +4939,17 @@
         <v>122</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5011,17 +4960,17 @@
         <v>122</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>211</v>
+        <v>123</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5032,17 +4981,17 @@
         <v>122</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>212</v>
+        <v>123</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5053,124 +5002,122 @@
         <v>122</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>123</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>215</v>
+        <v>123</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>217</v>
+        <v>86</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>218</v>
+        <v>123</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>174</v>
+        <v>90</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="F83" s="1"/>
       <c r="G83">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>146</v>
+        <v>203</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>147</v>
+        <v>92</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5178,20 +5125,20 @@
         <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>219</v>
+        <v>124</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5199,20 +5146,20 @@
         <v>6</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>220</v>
+        <v>97</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>221</v>
+        <v>123</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5220,20 +5167,20 @@
         <v>6</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>222</v>
+        <v>126</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5241,20 +5188,20 @@
         <v>6</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5262,20 +5209,20 @@
         <v>6</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>223</v>
+        <v>129</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5283,20 +5230,22 @@
         <v>6</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>223</v>
+        <v>94</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F90" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="G90">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5304,20 +5253,22 @@
         <v>6</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>223</v>
+        <v>47</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F91" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="G91">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5325,20 +5276,20 @@
         <v>6</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>224</v>
+        <v>120</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>225</v>
+        <v>123</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5346,20 +5297,20 @@
         <v>6</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>226</v>
+        <v>137</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5367,20 +5318,20 @@
         <v>6</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>226</v>
+        <v>139</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5388,20 +5339,20 @@
         <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>226</v>
+        <v>9</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5409,20 +5360,20 @@
         <v>6</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>226</v>
+        <v>80</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>228</v>
+        <v>123</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5430,162 +5381,177 @@
         <v>6</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F98" s="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="G98">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F99" s="1"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="G99">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>233</v>
+        <v>141</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F102" s="1"/>
+      <c r="G102">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F103" s="1"/>
+      <c r="G103">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B102" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G102">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="G103">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>242</v>
+      <c r="B104" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="G104">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G102"/>
+  <autoFilter ref="A1:G104"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the guidance text and modified issue text for the long stayer stuff
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -18,14 +18,14 @@
     <sheet name="All Checks" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$105</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="246">
   <si>
     <t>Source</t>
   </si>
@@ -753,13 +753,16 @@
     <t>This enrollment has been active without any updates to their Current Living Situation for longer than the days set for this Project Type in your Long Stayers settings on the Edit Local Settings tab. Please be sure that any CLS updates or project exits are reflected in HMIS.</t>
   </si>
   <si>
-    <t>Includes Services Only, Other, and Day Shelter</t>
-  </si>
-  <si>
     <t>Includes ES-NbN, Street Outreach, and Coordinated Entry</t>
   </si>
   <si>
     <t>4.12.1 - Information Date</t>
+  </si>
+  <si>
+    <t>Long Stayers (Local Settings)</t>
+  </si>
+  <si>
+    <t>This household has been housed in your project for a relatively long time compared to enrollments into the same project type in the rest of your system. If they have exited, please enter an Exit Date, otherwise consider using Move On Assistance funds. If they need to remain in the project, leave everything as is.</t>
   </si>
 </sst>
 </file>
@@ -1814,10 +1817,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD71"/>
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3282,7 +3285,7 @@
         <v>122</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>137</v>
@@ -3290,9 +3293,6 @@
       <c r="E73" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="G73">
         <v>102</v>
       </c>
@@ -3308,16 +3308,36 @@
         <v>240</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>241</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G74">
         <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G75">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3330,10 +3350,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5405,7 +5425,7 @@
         <v>122</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>137</v>
@@ -5413,9 +5433,6 @@
       <c r="E98" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="G98">
         <v>102</v>
       </c>
@@ -5431,37 +5448,36 @@
         <v>240</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>241</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G99">
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F100" s="1"/>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="G100">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5472,17 +5488,17 @@
         <v>122</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>216</v>
+        <v>141</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5493,17 +5509,17 @@
         <v>122</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>142</v>
+        <v>215</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>143</v>
+        <v>216</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>144</v>
+        <v>217</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5514,44 +5530,65 @@
         <v>122</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F104" s="1"/>
+      <c r="G104">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="B105" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F105" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G104">
+      <c r="G105">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G104"/>
+  <autoFilter ref="A1:G105"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated text for Long Stayers (Local Settings) guidance
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="248">
   <si>
     <t>Source</t>
   </si>
@@ -741,9 +741,6 @@
     <t>3.10 - Project Start Date, 3.917.3 - Prior Living Situation: Date  Homelessness Started</t>
   </si>
   <si>
-    <t>Long Stayers</t>
-  </si>
-  <si>
     <t>The number of days between Entry and the end of your CSV export exceeds the number of days in the Long Stayers settings for this project type. If this household has left the project, enter the Project Exit Date. If they are still active, do not change the data, but verify that your Coordinated Entry process is actively connecting this household to a permanent housing destination.</t>
   </si>
   <si>
@@ -763,6 +760,15 @@
   </si>
   <si>
     <t>This household has been housed in your project for a relatively long time compared to enrollments into the same project type in the rest of your system. If they have exited, please enter an Exit Date, otherwise consider using Move On Assistance funds. If they need to remain in the project, leave everything as is.</t>
+  </si>
+  <si>
+    <t>Long Stayers (Outliers)</t>
+  </si>
+  <si>
+    <t>ES, TH, SH, HP, and RRH project types are compared against the 98th percentile. PH, Housing Only, and Housing with Services project types are compared aginst the 99th percentile.</t>
+  </si>
+  <si>
+    <t>The number of days between Entry and the end of your CSV export exceeds the number of days in the Long Stayers settings for this project type. If this household has left the project, enter the Project Exit Date. If they are still active, do not change the data. It may be helpful to share this information with CE in accordance with your privacy policies to ensure this participant's needs are being met.</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1826,7 @@
   <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3285,13 +3291,13 @@
         <v>122</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>137</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G73">
         <v>102</v>
@@ -3305,16 +3311,16 @@
         <v>122</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="F74" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>242</v>
       </c>
       <c r="G74">
         <v>103</v>
@@ -3328,13 +3334,16 @@
         <v>122</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>137</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="G75">
         <v>104</v>
@@ -3352,8 +3361,8 @@
   </sheetPr>
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="C93" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5425,13 +5434,13 @@
         <v>122</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>137</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="G98">
         <v>102</v>
@@ -5445,16 +5454,16 @@
         <v>122</v>
       </c>
       <c r="C99" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E99" s="3" t="s">
+      <c r="F99" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>242</v>
       </c>
       <c r="G99">
         <v>103</v>
@@ -5468,13 +5477,16 @@
         <v>122</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>137</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="G100">
         <v>104</v>

</xml_diff>

<commit_message>
found a few issues pointed to the wrong rows (corrected)
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SilvermanA\eva\public-resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="6410" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="9495" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="File Structure" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="All Checks" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$106</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="250">
   <si>
     <t>Source</t>
   </si>
@@ -769,6 +769,12 @@
   </si>
   <si>
     <t>The number of days between Entry and the end of your CSV export exceeds the number of days in the Long Stayers settings for this project type. If this household has left the project, enter the Project Exit Date. If they are still active, do not change the data. It may be helpful to share this information with CE in accordance with your privacy policies to ensure this participant's needs are being met.</t>
+  </si>
+  <si>
+    <t>Don't Know/Refused Length of Stay</t>
+  </si>
+  <si>
+    <t>3.917.2 - Length of Stay in prior living situation</t>
   </si>
 </sst>
 </file>
@@ -804,11 +810,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1120,14 +1128,14 @@
       <selection activeCell="A2" sqref="A2:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1158,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1173,7 +1181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1193,7 +1201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1213,7 +1221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1233,7 +1241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1253,7 +1261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1273,7 +1281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1296,7 +1304,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1319,7 +1327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1339,7 +1347,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -1359,7 +1367,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1382,7 +1390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1402,7 +1410,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1422,7 +1430,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -1442,7 +1450,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -1462,7 +1470,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1482,7 +1490,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1502,7 +1510,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1522,7 +1530,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1542,7 +1550,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -1581,12 +1589,12 @@
       <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1609,7 +1617,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1632,7 +1640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1653,7 +1661,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1673,7 +1681,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1693,7 +1701,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1713,7 +1721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1733,7 +1741,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1753,7 +1761,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1773,7 +1781,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1793,7 +1801,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1829,12 +1837,12 @@
       <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1865,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1877,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1897,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1917,7 +1925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1937,7 +1945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1957,7 +1965,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1977,7 +1985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1997,7 +2005,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -2017,7 +2025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2037,7 +2045,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2065,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2077,7 +2085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2097,7 +2105,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -2117,7 +2125,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -2137,7 +2145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -2157,7 +2165,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -2177,7 +2185,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -2197,7 +2205,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -2217,7 +2225,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -2237,7 +2245,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -2257,7 +2265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -2277,7 +2285,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -2297,7 +2305,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2325,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
@@ -2337,7 +2345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
@@ -2357,7 +2365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
@@ -2377,7 +2385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
@@ -2397,7 +2405,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
@@ -2417,7 +2425,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
@@ -2437,7 +2445,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -2457,7 +2465,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>6</v>
       </c>
@@ -2477,7 +2485,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>6</v>
       </c>
@@ -2497,7 +2505,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
@@ -2517,7 +2525,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>6</v>
       </c>
@@ -2537,7 +2545,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2557,7 +2565,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
@@ -2577,7 +2585,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>6</v>
       </c>
@@ -2597,7 +2605,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>6</v>
       </c>
@@ -2617,7 +2625,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
@@ -2637,7 +2645,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
@@ -2657,7 +2665,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
@@ -2677,7 +2685,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
@@ -2697,7 +2705,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>6</v>
       </c>
@@ -2717,7 +2725,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>6</v>
       </c>
@@ -2737,7 +2745,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>6</v>
       </c>
@@ -2757,7 +2765,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>6</v>
       </c>
@@ -2777,7 +2785,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
@@ -2797,7 +2805,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>6</v>
       </c>
@@ -2817,7 +2825,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>6</v>
       </c>
@@ -2837,7 +2845,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>6</v>
       </c>
@@ -2857,7 +2865,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>6</v>
       </c>
@@ -2877,7 +2885,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>6</v>
       </c>
@@ -2897,7 +2905,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>6</v>
       </c>
@@ -2917,7 +2925,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
@@ -2937,7 +2945,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>6</v>
       </c>
@@ -2957,7 +2965,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>6</v>
       </c>
@@ -2977,7 +2985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>6</v>
       </c>
@@ -2997,7 +3005,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>6</v>
       </c>
@@ -3017,7 +3025,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>6</v>
       </c>
@@ -3037,7 +3045,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>6</v>
       </c>
@@ -3057,7 +3065,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>6</v>
       </c>
@@ -3077,7 +3085,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>6</v>
       </c>
@@ -3097,7 +3105,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>6</v>
       </c>
@@ -3117,7 +3125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>6</v>
       </c>
@@ -3140,7 +3148,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>6</v>
       </c>
@@ -3163,7 +3171,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>6</v>
       </c>
@@ -3183,7 +3191,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>6</v>
       </c>
@@ -3203,7 +3211,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>6</v>
       </c>
@@ -3223,7 +3231,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>6</v>
       </c>
@@ -3243,7 +3251,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>6</v>
       </c>
@@ -3263,7 +3271,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>6</v>
       </c>
@@ -3283,7 +3291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>6</v>
       </c>
@@ -3303,7 +3311,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>6</v>
       </c>
@@ -3326,7 +3334,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>6</v>
       </c>
@@ -3361,20 +3369,20 @@
   </sheetPr>
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C93" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="46.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3393,11 +3401,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3414,11 +3422,11 @@
         <v>10</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3435,11 +3443,11 @@
         <v>13</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3456,11 +3464,11 @@
         <v>15</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -3477,11 +3485,11 @@
         <v>17</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -3500,11 +3508,11 @@
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -3523,11 +3531,11 @@
       <c r="F7" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -3544,11 +3552,11 @@
         <v>28</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8">
+      <c r="G8" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -3565,11 +3573,11 @@
         <v>31</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9">
+      <c r="G9" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -3586,11 +3594,11 @@
         <v>33</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10">
+      <c r="G10" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -3607,11 +3615,11 @@
         <v>36</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -3628,11 +3636,11 @@
         <v>39</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -3651,11 +3659,11 @@
       <c r="F13" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -3674,52 +3682,52 @@
       <c r="F14" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>168</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>230</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>231</v>
+        <v>176</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G16">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+      <c r="G16" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -3727,20 +3735,20 @@
         <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>177</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3748,20 +3756,20 @@
         <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -3769,20 +3777,20 @@
         <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -3790,20 +3798,20 @@
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -3811,20 +3819,20 @@
         <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -3832,20 +3840,20 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -3853,20 +3861,20 @@
         <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>180</v>
+        <v>58</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -3874,20 +3882,20 @@
         <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -3895,20 +3903,20 @@
         <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -3916,20 +3924,20 @@
         <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -3937,20 +3945,20 @@
         <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G27" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -3958,20 +3966,20 @@
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -3979,20 +3987,20 @@
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G29" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -4000,20 +4008,20 @@
         <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G30" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -4021,20 +4029,20 @@
         <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G31" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -4042,20 +4050,20 @@
         <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F32" s="1"/>
-      <c r="G32">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G32" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -4063,20 +4071,20 @@
         <v>45</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -4084,104 +4092,104 @@
         <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="F37" s="1"/>
+      <c r="G37" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F37" s="1"/>
-      <c r="G37">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="F38" s="1"/>
-      <c r="G38">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G38" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
@@ -4189,20 +4197,20 @@
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F39" s="1"/>
-      <c r="G39">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G39" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
@@ -4210,757 +4218,757 @@
         <v>45</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G60" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="E63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F65" s="1"/>
+      <c r="G65" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="E66" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F42" s="1"/>
-      <c r="G42">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="E67" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F67" s="1"/>
+      <c r="G67" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F68" s="1"/>
+      <c r="G68" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F69" s="1"/>
+      <c r="G69" s="5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F72" s="1"/>
+      <c r="G72" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="1"/>
-      <c r="G43">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F44" s="1"/>
-      <c r="G44">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F45" s="1"/>
-      <c r="G45">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F46" s="1"/>
-      <c r="G46">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F47" s="1"/>
-      <c r="G47">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F49" s="1"/>
-      <c r="G49">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F50" s="1"/>
-      <c r="G50">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F51" s="1"/>
-      <c r="G51">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F52" s="1"/>
-      <c r="G52">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F53" s="1"/>
-      <c r="G53">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F54" s="1"/>
-      <c r="G54">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F55" s="1"/>
-      <c r="G55">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F56" s="1"/>
-      <c r="G56">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F57" s="1"/>
-      <c r="G57">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F58" s="1"/>
-      <c r="G58">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F59" s="1"/>
-      <c r="G59">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F60" s="2"/>
-      <c r="G60">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F61" s="1"/>
-      <c r="G61">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F62" s="1"/>
-      <c r="G62">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F63" s="1"/>
-      <c r="G63">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F64" s="1"/>
-      <c r="G64">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G65">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F66" s="1"/>
-      <c r="G66">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F67" s="1"/>
-      <c r="G67">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F68" s="1"/>
-      <c r="G68">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F69" s="1"/>
-      <c r="G69">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F70" s="1"/>
-      <c r="G70">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F71" s="1"/>
-      <c r="G71">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D72" s="1" t="s">
+      <c r="E73" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G73" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G74" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F72" s="1"/>
-      <c r="G72">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F73" s="1"/>
-      <c r="G73">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F74" s="1"/>
-      <c r="G74">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>123</v>
       </c>
       <c r="F75" s="1"/>
-      <c r="G75">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G75" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -4968,20 +4976,20 @@
         <v>122</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>195</v>
+        <v>136</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="F76" s="1"/>
-      <c r="G76">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G76" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>6</v>
       </c>
@@ -4989,20 +4997,20 @@
         <v>122</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>123</v>
+        <v>210</v>
       </c>
       <c r="F77" s="1"/>
-      <c r="G77">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G77" s="5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
@@ -5010,20 +5018,20 @@
         <v>122</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>123</v>
+        <v>211</v>
       </c>
       <c r="F78" s="1"/>
-      <c r="G78">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G78" s="5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
@@ -5031,576 +5039,577 @@
         <v>122</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>123</v>
       </c>
       <c r="F79" s="1"/>
-      <c r="G79">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G79" s="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F80" s="1"/>
+      <c r="G80" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F81" s="1"/>
+      <c r="G81" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F82" s="1"/>
+      <c r="G82" s="5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G83" s="5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F84" s="1"/>
+      <c r="G84" s="5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F85" s="1"/>
+      <c r="G85" s="5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F86" s="1"/>
+      <c r="G86" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F87" s="1"/>
+      <c r="G87" s="5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F88" s="1"/>
+      <c r="G88" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F89" s="1"/>
+      <c r="G89" s="5">
         <v>88</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F80" s="1"/>
-      <c r="G80">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F81" s="1"/>
-      <c r="G81">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F82" s="1"/>
-      <c r="G82">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D83" s="1" t="s">
+    </row>
+    <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F90" s="1"/>
+      <c r="G90" s="5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F91" s="1"/>
+      <c r="G91" s="5">
         <v>90</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F83" s="1"/>
-      <c r="G83">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D84" s="1" t="s">
+    </row>
+    <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F92" s="1"/>
+      <c r="G92" s="5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F93" s="1"/>
+      <c r="G93" s="5">
         <v>92</v>
       </c>
-      <c r="E84" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F84" s="1"/>
-      <c r="G84">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F85" s="1"/>
-      <c r="G85">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D86" s="1" t="s">
+    </row>
+    <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F94" s="1"/>
+      <c r="G94" s="5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F95" s="1"/>
+      <c r="G95" s="5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F96" s="1"/>
+      <c r="G96" s="5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F97" s="1"/>
+      <c r="G97" s="5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G98" s="5">
         <v>97</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F86" s="1"/>
-      <c r="G86">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F87" s="1"/>
-      <c r="G87">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F88" s="1"/>
-      <c r="G88">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F89" s="1"/>
-      <c r="G89">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G90">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G91">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F92" s="1"/>
-      <c r="G92">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D93" s="1" t="s">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G99" s="5">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G100" s="5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F101" s="1"/>
+      <c r="G101" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F102" s="1"/>
+      <c r="G102" s="5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F93" s="1"/>
-      <c r="G93">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F94" s="1"/>
-      <c r="G94">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F95" s="1"/>
-      <c r="G95">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F96" s="1"/>
-      <c r="G96">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F97" s="1"/>
-      <c r="G97">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D98" s="3" t="s">
+      <c r="E103" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F103" s="1"/>
+      <c r="G103" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G104" s="5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E98" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G98">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G99">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E100" s="3" t="s">
+      <c r="E105" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F100" s="3" t="s">
+      <c r="F105" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="G100">
+      <c r="G105" s="5">
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F101" s="1"/>
-      <c r="G101">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F102" s="1"/>
-      <c r="G102">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F103" s="1"/>
-      <c r="G103">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F104" s="1"/>
-      <c r="G104">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G105">
-        <v>82</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G105"/>
+  <autoFilter ref="A1:G106">
+    <sortState ref="A2:G100">
+      <sortCondition ref="G1"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:G106">
+    <sortCondition ref="G73"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated issues workbook to include additional check as requested
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="9495" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="File Structure" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="254">
   <si>
     <t>Source</t>
   </si>
@@ -775,6 +775,18 @@
   </si>
   <si>
     <t>3.917.2 - Length of Stay in prior living situation</t>
+  </si>
+  <si>
+    <t>Number of Months Homeless conflicts with Living Situation data</t>
+  </si>
+  <si>
+    <t>According to this client's assessment at Project Start, they experienced a single episode of homelessness in the three years prior to their enrollment and the approximate date homelessness started is known, but the total number of months they experienced homelessness prior to this enrollment is inconsistent with the given dates. Please double-check this information for consistency and accuracy.</t>
+  </si>
+  <si>
+    <t>Homelessness Start Date conflicts with Living Situation data</t>
+  </si>
+  <si>
+    <t>According to this client's assessment at Project Start, their Approximate Date Homeless was over three years ago, which would mean their Number of  Times Homeless would have to be 1 and their Number of Months Homeless would have to be "More than 12 months".</t>
   </si>
 </sst>
 </file>
@@ -810,13 +822,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3367,10 +3382,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4891,13 +4907,13 @@
         <v>122</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>129</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="5">
@@ -5599,6 +5615,23 @@
       </c>
       <c r="G105" s="5">
         <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G106" s="5">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
includes new enrollment v operating and enrollment v participating issues
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="279">
   <si>
     <t>Source</t>
   </si>
@@ -793,6 +793,75 @@
   </si>
   <si>
     <t>2.02A RRH SubType, 2.02.6 Project Type</t>
+  </si>
+  <si>
+    <t>Enrollment Crosses Operating Period</t>
+  </si>
+  <si>
+    <t>Enrollment After Participating Period</t>
+  </si>
+  <si>
+    <t>Enrollment Crosses Participating Start</t>
+  </si>
+  <si>
+    <t>Enrollment Before Participating Period</t>
+  </si>
+  <si>
+    <t>Enrollment Crosses Participating End</t>
+  </si>
+  <si>
+    <t>Enrollment Crosses Participation Period</t>
+  </si>
+  <si>
+    <t>Enrollment After Operating Period</t>
+  </si>
+  <si>
+    <t>Enrollment Crosses Operating Start</t>
+  </si>
+  <si>
+    <t>Enrollment Before Operating Period</t>
+  </si>
+  <si>
+    <t>Enrollment Crosses Operating End</t>
+  </si>
+  <si>
+    <t>This enrollment begins after the project stopped participating in HMIS. Please either correct your HMIS Participation End Date to include this enrollment, or this enrollment may be excluded from local and/or federal reporting.</t>
+  </si>
+  <si>
+    <t>Not considering this an Error because there may be PIT or survey data entered into HMIS that would flag here that admins may need for PIT reporting.</t>
+  </si>
+  <si>
+    <t>This enrollment begins before the project was participating in HMIS and either does not have an Exit or the Exit is after the project stopped participating. For reporting to work correctly, be sure your enrollment dates are within your HMIS participation dates.</t>
+  </si>
+  <si>
+    <t>This enrollment ends before the project started participating in HMIS. Please either correct your HMIS Participation Start Date to include this enrollment, or this enrollment may be excluded from local and/or federal reporting.</t>
+  </si>
+  <si>
+    <t>This enrollment ends after the project stopped participating in HMIS. For reporting to work correctly, be sure your enrollment dates are within your HMIS participation dates.</t>
+  </si>
+  <si>
+    <t>This enrollment begins before the project was participating in HMIS. For reporting to work correctly, be sure your enrollment dates are within your HMIS participation dates.</t>
+  </si>
+  <si>
+    <t>This enrollment begins after the project stopped operating. Please either correct your Operating End Date to include this enrollment or this enrollment may be excluded from local and/or federal reporting.</t>
+  </si>
+  <si>
+    <t>This enrollment begins before the project started operating. For reporting to work correctly, be sure your enrollment dates are within your project's operating dates.</t>
+  </si>
+  <si>
+    <t>This enrollment ends before the project started operating. Please either correct your Operating Start Date to include this enrollment or this enrollment may be excluded from local and/or federal reporting.</t>
+  </si>
+  <si>
+    <t>This enrollment ends after the project stopped operating. For reporting to work correctly, be sure your enrollment dates are within your HMIS participation dates.</t>
+  </si>
+  <si>
+    <t>This enrollment begins before the project was operating and either does not have an Exit or the Exit is after the project stopped operating. For reporting to work correctly, be sure your enrollment dates are within your project's operating dates.</t>
+  </si>
+  <si>
+    <t>2.08.1 HMIS Participation Type, 2.08.2 HMIS Participating Start, 2.08.3 HMIS Participating End</t>
+  </si>
+  <si>
+    <t>2.02.3 Operating Start Date, 2.02.4 Operating End Date</t>
   </si>
 </sst>
 </file>
@@ -3392,11 +3461,11 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5483,6 +5552,212 @@
       </c>
       <c r="G107" s="5">
         <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G108" s="5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G109" s="5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G110" s="5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G111" s="5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="G112" s="5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="G113" s="5">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G114" s="5">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G115" s="5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G116" s="5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G117" s="5">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved issue from old way to new way
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="9495" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="File Structure" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="All Checks" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$117</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="283">
   <si>
     <t>Source</t>
   </si>
@@ -862,6 +862,18 @@
   </si>
   <si>
     <t>2.02.3 Operating Start Date, 2.02.4 Operating End Date</t>
+  </si>
+  <si>
+    <t>Missing Destination Subsidy Type</t>
+  </si>
+  <si>
+    <t>If a client exits to Rental by Client, the user must record the Subsidy Type.</t>
+  </si>
+  <si>
+    <t>3.12.1 - Destination, 3.12.A - Destination Subsidy Type</t>
+  </si>
+  <si>
+    <t>3.12.1 - Destination</t>
   </si>
 </sst>
 </file>
@@ -3458,14 +3470,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3501,7 +3513,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -3521,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -3541,7 +3553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -3561,7 +3573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3604,7 +3616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -3627,7 +3639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -3647,7 +3659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -3667,7 +3679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -3687,7 +3699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -3707,7 +3719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -3727,7 +3739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -3750,7 +3762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -3773,7 +3785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -3793,7 +3805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -3813,7 +3825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
@@ -3833,7 +3845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -3853,7 +3865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -3873,7 +3885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -3893,7 +3905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -3913,7 +3925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
@@ -3933,7 +3945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -3953,7 +3965,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -3973,8 +3985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -3994,7 +4005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
@@ -4014,7 +4025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
@@ -4034,7 +4045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -4054,7 +4065,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
@@ -4074,7 +4085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
@@ -4094,7 +4105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>6</v>
       </c>
@@ -4114,7 +4125,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>6</v>
       </c>
@@ -4134,7 +4145,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
@@ -4154,7 +4165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
@@ -4174,7 +4185,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>6</v>
       </c>
@@ -4194,7 +4205,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>6</v>
       </c>
@@ -4214,8 +4225,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>6</v>
       </c>
@@ -4235,7 +4245,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>6</v>
       </c>
@@ -4255,7 +4265,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>6</v>
       </c>
@@ -4275,7 +4285,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>6</v>
       </c>
@@ -4356,7 +4366,6 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>18</v>
@@ -4377,7 +4386,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>23</v>
       </c>
@@ -4400,7 +4409,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>23</v>
       </c>
@@ -4420,7 +4429,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
@@ -4440,7 +4449,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -4460,7 +4469,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -4480,7 +4489,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>23</v>
       </c>
@@ -4500,7 +4509,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -4520,7 +4529,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>23</v>
       </c>
@@ -4531,7 +4540,7 @@
         <v>119</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>120</v>
+        <v>282</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>190</v>
@@ -4540,7 +4549,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>23</v>
       </c>
@@ -4560,7 +4569,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>6</v>
       </c>
@@ -4580,7 +4589,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
@@ -4600,7 +4609,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
@@ -4620,7 +4629,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>6</v>
       </c>
@@ -4631,7 +4640,7 @@
         <v>196</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>120</v>
+        <v>282</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>123</v>
@@ -4640,7 +4649,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>6</v>
       </c>
@@ -4660,7 +4669,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>6</v>
       </c>
@@ -4680,8 +4689,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>6</v>
       </c>
@@ -4701,7 +4709,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>6</v>
       </c>
@@ -4721,7 +4729,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>6</v>
       </c>
@@ -4741,7 +4749,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>6</v>
       </c>
@@ -4761,7 +4769,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>6</v>
       </c>
@@ -4781,7 +4789,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
@@ -4801,7 +4809,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>6</v>
       </c>
@@ -4821,7 +4829,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>6</v>
       </c>
@@ -4841,7 +4849,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>6</v>
       </c>
@@ -4861,7 +4869,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>6</v>
       </c>
@@ -4884,7 +4892,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>6</v>
       </c>
@@ -4904,7 +4912,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>6</v>
       </c>
@@ -4924,7 +4932,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>6</v>
       </c>
@@ -4944,7 +4952,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>6</v>
       </c>
@@ -4964,7 +4972,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>6</v>
       </c>
@@ -4984,7 +4992,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>6</v>
       </c>
@@ -5064,7 +5072,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>23</v>
       </c>
@@ -5107,7 +5115,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>6</v>
       </c>
@@ -5127,7 +5135,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>6</v>
       </c>
@@ -5147,7 +5155,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>6</v>
       </c>
@@ -5167,7 +5175,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>6</v>
       </c>
@@ -5187,7 +5195,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
@@ -5207,7 +5215,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>6</v>
       </c>
@@ -5227,7 +5235,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>6</v>
       </c>
@@ -5247,7 +5255,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>6</v>
       </c>
@@ -5267,7 +5275,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>6</v>
       </c>
@@ -5287,7 +5295,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>6</v>
       </c>
@@ -5307,7 +5315,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>6</v>
       </c>
@@ -5327,7 +5335,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>6</v>
       </c>
@@ -5347,7 +5355,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>6</v>
       </c>
@@ -5367,7 +5375,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>6</v>
       </c>
@@ -5387,7 +5395,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>23</v>
       </c>
@@ -5407,7 +5415,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>6</v>
       </c>
@@ -5427,7 +5435,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>6</v>
       </c>
@@ -5447,7 +5455,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>23</v>
       </c>
@@ -5467,7 +5475,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>6</v>
       </c>
@@ -5487,7 +5495,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>6</v>
       </c>
@@ -5510,7 +5518,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>6</v>
       </c>
@@ -5533,7 +5541,6 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>18</v>
@@ -5760,13 +5767,28 @@
         <v>120</v>
       </c>
     </row>
+    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="G118" s="5">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G106">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="pdde"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:G117">
     <sortState ref="A2:G100">
       <sortCondition ref="G1"/>
     </sortState>

</xml_diff>

<commit_message>
changed incorrectly capitalized column names to Errors
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -18,14 +18,14 @@
     <sheet name="All Checks" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$113</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="284">
   <si>
     <t>Source</t>
   </si>
@@ -874,6 +874,9 @@
   </si>
   <si>
     <t>3.12.1 - Destination</t>
+  </si>
+  <si>
+    <t>If the column is considered High Priority, this will be a High Priority issue. Otherwise, this will be considered an Error.</t>
   </si>
 </sst>
 </file>
@@ -3473,11 +3476,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G118"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3624,19 +3627,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>175</v>
+        <v>31</v>
       </c>
       <c r="G7" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3659,27 +3659,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="G9" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -3687,19 +3687,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>27</v>
+        <v>230</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>33</v>
+        <v>231</v>
       </c>
       <c r="G10" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -3707,16 +3707,19 @@
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>174</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="G11" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3724,22 +3727,25 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>38</v>
+        <v>174</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="G12" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -3747,19 +3753,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>174</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>175</v>
       </c>
       <c r="G13" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3767,7 +3773,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>43</v>
@@ -3778,11 +3784,8 @@
       <c r="E14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>175</v>
-      </c>
       <c r="G14" s="5">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3985,6 +3988,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" s="5">
+        <v>25</v>
+      </c>
+    </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>6</v>
@@ -3993,16 +4016,16 @@
         <v>45</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G26" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4013,16 +4036,16 @@
         <v>45</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>65</v>
+        <v>250</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G27" s="5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4033,16 +4056,16 @@
         <v>45</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>250</v>
+        <v>69</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G28" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4053,16 +4076,16 @@
         <v>45</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G29" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4073,19 +4096,19 @@
         <v>45</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G30" s="5">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
@@ -4093,19 +4116,19 @@
         <v>45</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G31" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>6</v>
       </c>
@@ -4113,19 +4136,19 @@
         <v>45</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G32" s="5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>6</v>
       </c>
@@ -4133,19 +4156,19 @@
         <v>45</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="G33" s="5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
@@ -4153,16 +4176,16 @@
         <v>45</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G34" s="5">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -4173,19 +4196,19 @@
         <v>45</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>183</v>
       </c>
       <c r="G35" s="5">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>6</v>
       </c>
@@ -4193,16 +4216,16 @@
         <v>45</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>83</v>
+        <v>251</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="G36" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4213,16 +4236,36 @@
         <v>45</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>251</v>
+        <v>89</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>155</v>
       </c>
       <c r="G37" s="5">
-        <v>36</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G38" s="5">
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4233,19 +4276,19 @@
         <v>45</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="G39" s="5">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>6</v>
       </c>
@@ -4253,59 +4296,60 @@
         <v>45</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="G40" s="5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>95</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F41" s="6"/>
       <c r="G41" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G42" s="5">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>18</v>
       </c>
@@ -4313,20 +4357,19 @@
         <v>45</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F43" s="6"/>
+        <v>106</v>
+      </c>
       <c r="G43" s="5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>18</v>
       </c>
@@ -4334,56 +4377,79 @@
         <v>45</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G44" s="5">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="G45" s="5">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="G47" s="5">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -4394,22 +4460,19 @@
         <v>45</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>38</v>
+        <v>282</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="G48" s="5">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>23</v>
       </c>
@@ -4417,19 +4480,19 @@
         <v>45</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>174</v>
+        <v>80</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>44</v>
+        <v>187</v>
       </c>
       <c r="G49" s="5">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
@@ -4437,19 +4500,19 @@
         <v>45</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G50" s="5">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -4457,19 +4520,19 @@
         <v>45</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G51" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -4477,96 +4540,96 @@
         <v>45</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G52" s="5">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>117</v>
+        <v>172</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>74</v>
+        <v>235</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="G53" s="5">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>118</v>
+        <v>193</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>189</v>
+        <v>123</v>
       </c>
       <c r="G54" s="5">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>119</v>
+        <v>194</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>282</v>
+        <v>179</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>190</v>
+        <v>123</v>
       </c>
       <c r="G55" s="5">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>121</v>
+        <v>180</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
       <c r="G56" s="5">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4577,16 +4640,16 @@
         <v>122</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>181</v>
+        <v>282</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G57" s="5">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4597,16 +4660,16 @@
         <v>122</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>179</v>
+        <v>82</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G58" s="5">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4617,36 +4680,39 @@
         <v>122</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G59" s="5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>196</v>
+        <v>24</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>282</v>
+        <v>174</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>123</v>
+        <v>25</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="G60" s="5">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4657,16 +4723,16 @@
         <v>122</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>197</v>
+        <v>252</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G61" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4677,16 +4743,36 @@
         <v>122</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G62" s="5">
-        <v>61</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G63" s="5">
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4697,16 +4783,16 @@
         <v>122</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>252</v>
+        <v>203</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G64" s="5">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4717,16 +4803,16 @@
         <v>122</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G65" s="5">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4737,19 +4823,19 @@
         <v>122</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G66" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>6</v>
       </c>
@@ -4757,19 +4843,19 @@
         <v>122</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>203</v>
+        <v>125</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="G67" s="5">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>6</v>
       </c>
@@ -4777,16 +4863,16 @@
         <v>122</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>204</v>
+        <v>127</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>123</v>
+        <v>207</v>
       </c>
       <c r="G68" s="5">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4797,56 +4883,59 @@
         <v>122</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>205</v>
+        <v>128</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="E69" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G69" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G70" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G69" s="5">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="G70" s="5">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>207</v>
-      </c>
       <c r="G71" s="5">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4857,19 +4946,19 @@
         <v>122</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="G72" s="5">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>6</v>
       </c>
@@ -4877,22 +4966,19 @@
         <v>122</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="G73" s="5">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>6</v>
       </c>
@@ -4900,139 +4986,139 @@
         <v>122</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>248</v>
+        <v>209</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>249</v>
+        <v>139</v>
       </c>
       <c r="E74" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G74" s="5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G75" s="5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E76" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G74" s="5">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G75" s="5">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="G76" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="G77" s="5">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="D78" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G78" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G79" s="5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G80" s="5">
         <v>9</v>
       </c>
-      <c r="E78" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="G78" s="5">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G79" s="5">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G80" s="5">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>18</v>
       </c>
@@ -5040,79 +5126,76 @@
         <v>122</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>215</v>
+        <v>146</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>216</v>
+        <v>147</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>217</v>
+        <v>148</v>
       </c>
       <c r="G81" s="5">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G82" s="5">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>145</v>
+        <v>220</v>
       </c>
       <c r="G83" s="5">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G84" s="5">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5123,19 +5206,19 @@
         <v>45</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G85" s="5">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>6</v>
       </c>
@@ -5143,19 +5226,19 @@
         <v>45</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>220</v>
+        <v>157</v>
       </c>
       <c r="G86" s="5">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>6</v>
       </c>
@@ -5163,19 +5246,19 @@
         <v>45</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G87" s="5">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>6</v>
       </c>
@@ -5183,19 +5266,19 @@
         <v>45</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>222</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G88" s="5">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
@@ -5203,16 +5286,16 @@
         <v>45</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>157</v>
+        <v>224</v>
       </c>
       <c r="G89" s="5">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5223,39 +5306,39 @@
         <v>45</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E90" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G90" s="5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G90" s="5">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="G91" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>6</v>
       </c>
@@ -5263,19 +5346,19 @@
         <v>45</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G92" s="5">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>6</v>
       </c>
@@ -5283,16 +5366,16 @@
         <v>45</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>155</v>
+        <v>227</v>
       </c>
       <c r="G93" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5303,16 +5386,16 @@
         <v>45</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G94" s="5">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -5323,39 +5406,39 @@
         <v>45</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G95" s="5">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>165</v>
+        <v>34</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>227</v>
+        <v>36</v>
       </c>
       <c r="G96" s="5">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>6</v>
       </c>
@@ -5363,79 +5446,82 @@
         <v>45</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>155</v>
+        <v>233</v>
       </c>
       <c r="G97" s="5">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="G98" s="5">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>168</v>
+        <v>243</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>230</v>
+        <v>137</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="G99" s="5">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>169</v>
+        <v>239</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>233</v>
+        <v>240</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="G100" s="5">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>6</v>
       </c>
@@ -5443,39 +5529,42 @@
         <v>122</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>170</v>
+        <v>245</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>234</v>
+        <v>137</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>171</v>
+        <v>244</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="G101" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>172</v>
+        <v>253</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>173</v>
+        <v>254</v>
       </c>
       <c r="G102" s="5">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>6</v>
       </c>
@@ -5483,42 +5572,42 @@
         <v>122</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>137</v>
+        <v>277</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>247</v>
+        <v>266</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="G103" s="5">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="G104" s="5">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>6</v>
       </c>
@@ -5526,39 +5615,59 @@
         <v>122</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>137</v>
+        <v>277</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="G105" s="5">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G106" s="5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="G107" s="5">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5566,25 +5675,22 @@
         <v>6</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="G108" s="5">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>6</v>
       </c>
@@ -5592,16 +5698,16 @@
         <v>45</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="G109" s="5">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5609,25 +5715,22 @@
         <v>6</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="F110" s="4" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="G110" s="5">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>6</v>
       </c>
@@ -5635,16 +5738,16 @@
         <v>45</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="G111" s="5">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -5655,19 +5758,19 @@
         <v>45</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="G112" s="5">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>6</v>
       </c>
@@ -5675,122 +5778,22 @@
         <v>45</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="G113" s="5">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E114" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="G114" s="5">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E115" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="G115" s="5">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="G116" s="5">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="G117" s="5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="G118" s="5">
         <v>121</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G117">
-    <sortState ref="A2:G100">
-      <sortCondition ref="G1"/>
+  <autoFilter ref="A1:G113">
+    <sortState ref="A7:G99">
+      <sortCondition ref="C1:C114"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:G106">

</xml_diff>

<commit_message>
updated check text and added new check to EvaChecks.xlsx
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SilvermanA\eva\public-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="9495" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21080" windowHeight="9500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="File Structure" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="All Checks" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'All Checks'!$A$1:$G$114</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="288">
   <si>
     <t>Source</t>
   </si>
@@ -877,6 +877,18 @@
   </si>
   <si>
     <t>If the column is considered High Priority, this will be a High Priority issue. Otherwise, this will be considered an Error.</t>
+  </si>
+  <si>
+    <t>Homelessness Start Date conflicts with Living Situation data</t>
+  </si>
+  <si>
+    <t>According to this client's assessment at Project Start, their Approximate Date Homeless was over three years ago, which would mean their Number of  Times Homeless would have to be 1 and their Number of Months Homeless would have to be "More than 12 months".</t>
+  </si>
+  <si>
+    <t>Number of Months Homeless conflicts with Living Situation data</t>
+  </si>
+  <si>
+    <t>According to this client's assessment at Project Start, they experienced a single episode of homelessness in the three years prior to their enrollment and the approximate date homelessness started is known, but the total number of months they experienced homelessness prior to this enrollment is inconsistent with the given dates. Please double-check this information for consistency and accuracy.</t>
   </si>
 </sst>
 </file>
@@ -1237,14 +1249,14 @@
       <selection activeCell="A2" sqref="A2:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1279,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1350,7 +1362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1413,7 +1425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1456,7 +1468,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -1476,7 +1488,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +1511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1519,7 +1531,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1539,7 +1551,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -1559,7 +1571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -1579,7 +1591,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1599,7 +1611,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1619,7 +1631,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1659,7 +1671,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -1698,12 +1710,12 @@
       <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1738,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1749,7 +1761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1770,7 +1782,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1790,7 +1802,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1810,7 +1822,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1850,7 +1862,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1870,7 +1882,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1890,7 +1902,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1910,7 +1922,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1946,12 +1958,12 @@
       <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +1986,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1994,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2014,7 +2026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2034,7 +2046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2054,7 +2066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2074,7 +2086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2094,7 +2106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -2134,7 +2146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -2174,7 +2186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -2214,7 +2226,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -2234,7 +2246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -2254,7 +2266,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -2274,7 +2286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -2294,7 +2306,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -2314,7 +2326,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -2334,7 +2346,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -2354,7 +2366,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
@@ -2374,7 +2386,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -2394,7 +2406,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -2414,7 +2426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
@@ -2434,7 +2446,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
@@ -2454,7 +2466,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
@@ -2474,7 +2486,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
@@ -2494,7 +2506,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
@@ -2554,7 +2566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -2574,7 +2586,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>6</v>
       </c>
@@ -2594,7 +2606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>6</v>
       </c>
@@ -2614,7 +2626,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
@@ -2634,7 +2646,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>6</v>
       </c>
@@ -2654,7 +2666,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2674,7 +2686,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
@@ -2694,7 +2706,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>6</v>
       </c>
@@ -2714,7 +2726,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>6</v>
       </c>
@@ -2734,7 +2746,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
@@ -2754,7 +2766,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
@@ -2774,7 +2786,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
@@ -2794,7 +2806,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
@@ -2814,7 +2826,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>6</v>
       </c>
@@ -2834,7 +2846,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>6</v>
       </c>
@@ -2854,7 +2866,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>6</v>
       </c>
@@ -2874,7 +2886,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>6</v>
       </c>
@@ -2894,7 +2906,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
@@ -2914,7 +2926,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>6</v>
       </c>
@@ -2934,7 +2946,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>6</v>
       </c>
@@ -2954,7 +2966,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>6</v>
       </c>
@@ -2974,7 +2986,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>6</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>6</v>
       </c>
@@ -3014,7 +3026,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>6</v>
       </c>
@@ -3034,7 +3046,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
@@ -3054,7 +3066,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>6</v>
       </c>
@@ -3074,7 +3086,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>6</v>
       </c>
@@ -3094,7 +3106,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>6</v>
       </c>
@@ -3114,7 +3126,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>6</v>
       </c>
@@ -3134,7 +3146,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>6</v>
       </c>
@@ -3154,7 +3166,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>6</v>
       </c>
@@ -3174,7 +3186,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>6</v>
       </c>
@@ -3194,7 +3206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>6</v>
       </c>
@@ -3214,7 +3226,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>6</v>
       </c>
@@ -3234,7 +3246,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>6</v>
       </c>
@@ -3257,7 +3269,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>6</v>
       </c>
@@ -3280,7 +3292,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>6</v>
       </c>
@@ -3300,7 +3312,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>6</v>
       </c>
@@ -3320,7 +3332,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>6</v>
       </c>
@@ -3340,7 +3352,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>6</v>
       </c>
@@ -3360,7 +3372,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>6</v>
       </c>
@@ -3380,7 +3392,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>6</v>
       </c>
@@ -3400,7 +3412,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>6</v>
       </c>
@@ -3420,7 +3432,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>6</v>
       </c>
@@ -3443,7 +3455,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>6</v>
       </c>
@@ -3476,24 +3488,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="4" customWidth="1"/>
-    <col min="5" max="6" width="57.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="2" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="57.81640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="5"/>
+    <col min="8" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3516,7 +3528,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -3536,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -3556,7 +3568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -3576,7 +3588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3596,7 +3608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -3619,7 +3631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -3639,7 +3651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -3659,7 +3671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -3679,7 +3691,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -3699,7 +3711,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -3722,7 +3734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -3745,7 +3757,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -3768,7 +3780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -3788,7 +3800,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -3808,7 +3820,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -3828,7 +3840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
@@ -3848,7 +3860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -3868,7 +3880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -3888,7 +3900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -3908,7 +3920,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -3928,7 +3940,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
@@ -3948,7 +3960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -3968,7 +3980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -3988,7 +4000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
@@ -4008,7 +4020,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -4028,7 +4040,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
@@ -4048,7 +4060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
@@ -4068,7 +4080,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -4088,7 +4100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
@@ -4108,7 +4120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
@@ -4128,7 +4140,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>6</v>
       </c>
@@ -4148,7 +4160,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>6</v>
       </c>
@@ -4168,7 +4180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>6</v>
       </c>
@@ -4188,7 +4200,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
@@ -4208,7 +4220,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>6</v>
       </c>
@@ -4228,7 +4240,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>6</v>
       </c>
@@ -4248,7 +4260,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>6</v>
       </c>
@@ -4268,7 +4280,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>6</v>
       </c>
@@ -4288,7 +4300,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>6</v>
       </c>
@@ -4308,7 +4320,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>18</v>
       </c>
@@ -4329,7 +4341,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>18</v>
       </c>
@@ -4349,7 +4361,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>18</v>
       </c>
@@ -4369,7 +4381,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>18</v>
       </c>
@@ -4389,7 +4401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>23</v>
       </c>
@@ -4409,7 +4421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>23</v>
       </c>
@@ -4432,7 +4444,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>23</v>
       </c>
@@ -4452,7 +4464,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>23</v>
       </c>
@@ -4472,7 +4484,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>23</v>
       </c>
@@ -4492,7 +4504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
@@ -4512,7 +4524,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -4532,7 +4544,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -4552,7 +4564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>23</v>
       </c>
@@ -4572,7 +4584,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>6</v>
       </c>
@@ -4592,7 +4604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>6</v>
       </c>
@@ -4612,7 +4624,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>6</v>
       </c>
@@ -4632,7 +4644,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>6</v>
       </c>
@@ -4652,7 +4664,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
@@ -4672,7 +4684,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
@@ -4692,7 +4704,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>23</v>
       </c>
@@ -4715,7 +4727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>6</v>
       </c>
@@ -4735,7 +4747,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>6</v>
       </c>
@@ -4755,7 +4767,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>6</v>
       </c>
@@ -4775,7 +4787,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>6</v>
       </c>
@@ -4795,7 +4807,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>6</v>
       </c>
@@ -4815,7 +4827,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +4847,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>6</v>
       </c>
@@ -4855,7 +4867,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>6</v>
       </c>
@@ -4875,7 +4887,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
@@ -4883,19 +4895,19 @@
         <v>122</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>128</v>
+        <v>286</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>129</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>208</v>
+        <v>287</v>
       </c>
       <c r="G69" s="5">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>6</v>
       </c>
@@ -4918,7 +4930,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>6</v>
       </c>
@@ -4938,7 +4950,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>6</v>
       </c>
@@ -4958,7 +4970,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>6</v>
       </c>
@@ -4978,7 +4990,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>6</v>
       </c>
@@ -4998,7 +5010,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>6</v>
       </c>
@@ -5018,7 +5030,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>6</v>
       </c>
@@ -5038,7 +5050,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>18</v>
       </c>
@@ -5058,7 +5070,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>18</v>
       </c>
@@ -5078,7 +5090,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>18</v>
       </c>
@@ -5098,7 +5110,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>23</v>
       </c>
@@ -5118,7 +5130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>18</v>
       </c>
@@ -5138,7 +5150,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>6</v>
       </c>
@@ -5158,7 +5170,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>6</v>
       </c>
@@ -5178,7 +5190,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>6</v>
       </c>
@@ -5198,7 +5210,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>6</v>
       </c>
@@ -5218,7 +5230,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>6</v>
       </c>
@@ -5238,7 +5250,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>6</v>
       </c>
@@ -5258,7 +5270,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>6</v>
       </c>
@@ -5278,7 +5290,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
@@ -5298,7 +5310,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>6</v>
       </c>
@@ -5318,7 +5330,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>6</v>
       </c>
@@ -5338,7 +5350,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>6</v>
       </c>
@@ -5358,7 +5370,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>6</v>
       </c>
@@ -5378,7 +5390,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>6</v>
       </c>
@@ -5398,7 +5410,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>6</v>
       </c>
@@ -5418,7 +5430,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>23</v>
       </c>
@@ -5438,7 +5450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>6</v>
       </c>
@@ -5458,7 +5470,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>6</v>
       </c>
@@ -5478,7 +5490,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>6</v>
       </c>
@@ -5498,7 +5510,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>6</v>
       </c>
@@ -5521,7 +5533,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>6</v>
       </c>
@@ -5544,7 +5556,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>18</v>
       </c>
@@ -5564,7 +5576,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>6</v>
       </c>
@@ -5587,7 +5599,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>6</v>
       </c>
@@ -5607,7 +5619,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>6</v>
       </c>
@@ -5630,7 +5642,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>6</v>
       </c>
@@ -5650,7 +5662,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>6</v>
       </c>
@@ -5670,7 +5682,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
         <v>6</v>
       </c>
@@ -5690,7 +5702,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>6</v>
       </c>
@@ -5710,7 +5722,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>6</v>
       </c>
@@ -5730,7 +5742,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>6</v>
       </c>
@@ -5750,7 +5762,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>6</v>
       </c>
@@ -5770,7 +5782,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
         <v>6</v>
       </c>
@@ -5790,12 +5802,25 @@
         <v>121</v>
       </c>
     </row>
+    <row r="114" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="G114" s="5">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G113">
-    <sortState ref="A7:G99">
-      <sortCondition ref="C1:C114"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G114"/>
   <sortState ref="A2:G106">
     <sortCondition ref="G73"/>
   </sortState>

</xml_diff>

<commit_message>
trying to resolve conflicts with FY24 dev
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -885,10 +885,10 @@
     <t>According to this client's assessment at Project Start, their Approximate Date Homeless was over three years ago, which would mean their Number of  Times Homeless would have to be 1 and their Number of Months Homeless would have to be "More than 12 months".</t>
   </si>
   <si>
-    <t>Number of Months Homeless conflicts with Living Situation data</t>
-  </si>
-  <si>
-    <t>According to this client's assessment at Project Start, they experienced a single episode of homelessness in the three years prior to their enrollment and the approximate date homelessness started is known, but the total number of months they experienced homelessness prior to this enrollment is inconsistent with the given dates. Please double-check this information for consistency and accuracy.</t>
+    <t>3.04 - Race/Ethnicity</t>
+  </si>
+  <si>
+    <t>You have at least one active referral that has been active without a Result Date for longer than the days set in your Local Settings on the Edit Local Settings tab.</t>
   </si>
 </sst>
 </file>
@@ -3491,8 +3491,8 @@
   <dimension ref="A1:G114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4231,7 +4231,7 @@
         <v>251</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>86</v>
+        <v>286</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>155</v>
@@ -4895,13 +4895,13 @@
         <v>122</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>286</v>
+        <v>128</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>129</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>287</v>
+        <v>208</v>
       </c>
       <c r="G69" s="5">
         <v>71</v>
@@ -5484,7 +5484,7 @@
         <v>234</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>171</v>
+        <v>287</v>
       </c>
       <c r="G98" s="5">
         <v>100</v>

</xml_diff>

<commit_message>
reordered and added High Priority file structure issues, removed three rows for which there was no match in the code because they were renamed/reworked or they don't exist in the new branch.
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\rstudio-export (10)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="9495"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="EvaChecks"/>
+    <sheet name="EvaChecks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">EvaChecks!$A$1:$G$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">EvaChecks!$A$1:$G$111</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="4264353701"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="273">
   <si>
     <t>Type</t>
   </si>
@@ -427,15 +432,6 @@
     <t>This client's Exit Date is a date in the future. Please enter the exact date the client left your program. If this client has not yet exited, delete the Exit and then enter the Exit Date once the client is no longer in your program.</t>
   </si>
   <si>
-    <t>Exit After Project's Operating End Date</t>
-  </si>
-  <si>
-    <t>3.11 - Project Exit Date, 2.02.4 - Operating Exit Date</t>
-  </si>
-  <si>
-    <t>This enrollment is active outside of the project's operating start and end dates. Please reconcile this by either correcting the Exit Date(s) or the project's Operating End Date.</t>
-  </si>
-  <si>
     <t>Project Exit Before Start</t>
   </si>
   <si>
@@ -631,15 +627,6 @@
     <t>Projects no longer in operation must have an Operating End Date. Please verify if the project is still in operation and, if not, add in the Operating End Date.</t>
   </si>
   <si>
-    <t>Non-HMIS-Participating Discrepancy</t>
-  </si>
-  <si>
-    <t>2.02.7 - Project Information: HMIS Participating Project</t>
-  </si>
-  <si>
-    <t>There are enrollments entered in this non-HMIS-participating project. Verify that the Non-HMIS-participating status of this project is correct.</t>
-  </si>
-  <si>
     <t>Inventory Start Precedes Operating Start</t>
   </si>
   <si>
@@ -658,15 +645,6 @@
     <t>Any project with active beds in the reporting period should have one or more active clients in the reporting period.</t>
   </si>
   <si>
-    <t>Entry Precedes Operating Start</t>
-  </si>
-  <si>
-    <t>2.02.3 - Operating Start Date, 3.10 - Project Start Date</t>
-  </si>
-  <si>
-    <t>This enrollment is active outside of the project's operating start and end dates. Please reconcile this by either correcting the Entry Date or the project's Operating Start Date.</t>
-  </si>
-  <si>
     <t>Enrollment After Participating Period</t>
   </si>
   <si>
@@ -824,13 +802,51 @@
   </si>
   <si>
     <t>Don't Know/Refused War(s)</t>
+  </si>
+  <si>
+    <t>Your zip file is misstructured</t>
+  </si>
+  <si>
+    <t>You may have uploaded the wrong dataset</t>
+  </si>
+  <si>
+    <t>Your HMIS CSV Export is out of date</t>
+  </si>
+  <si>
+    <t>Missing Files</t>
+  </si>
+  <si>
+    <t>You uploaded an unhashed data set</t>
+  </si>
+  <si>
+    <t>Determined from file metadata</t>
+  </si>
+  <si>
+    <t>Export.csv - CSVVersion column</t>
+  </si>
+  <si>
+    <t>Export.csv - HashStatus, Client.csv - FirstName</t>
+  </si>
+  <si>
+    <t>It looks like you may have unzipped your HMIS csv because the individual csv files are contained within a subdirectory.</t>
+  </si>
+  <si>
+    <t>Your upload does not contain an Export.csv file which means you either uploaded something other than an HMIS CSV export or your export does not contain all the files outlined in the HMIS CSV Export  specifications. Be sure that you haven't accidentally uploaded an APR or an LSA. If you are not sure how to run the hashed HMIS CSV Export in your HMIS, please contact your HMIS vendor.</t>
+  </si>
+  <si>
+    <t>It looks like you either uploaded an FY2022 HMIS CSV Export or your vendor needs to update your Export.csv's CSV Version. If you are not sure how to obtain an FY2024 HMIS CSV Export in your HMIS, please contact your HMIS vendor.</t>
+  </si>
+  <si>
+    <t>You have uploaded an unhashed version of the HMIS CSV Export. If you are not sure how to run the hashed HMIS CSV Export in your  HMIS, please contact your HMIS vendor.</t>
+  </si>
+  <si>
+    <t>Your zip file appears to be missing the following files: [files listed] You either uploaded something other than an HMIS CSV export or your export does not contain all the files outlined in the HMIS CSV Export specifications. If you are not sure how to run the hashed HMIS CSV Export in your HMIS, please contact your HMIS vendor.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,32 +889,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -909,10 +933,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -950,71 +974,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1042,7 +1066,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1065,11 +1089,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1078,13 +1102,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1094,7 +1118,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1103,7 +1127,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1112,7 +1136,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1120,10 +1144,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1192,24 +1216,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +1256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1240,20 +1264,20 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1261,20 +1285,20 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="3">
-        <v>101</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1282,20 +1306,20 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1303,20 +1327,22 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1324,20 +1350,22 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G6" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1345,20 +1373,20 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="3">
-        <v>98</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1366,20 +1394,20 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>265</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="G8" s="7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1387,22 +1415,20 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1410,22 +1436,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1433,129 +1459,125 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>261</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>265</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>269</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="G13" s="7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>264</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>48</v>
+        <v>267</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="G14" s="7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>262</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>266</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="G15" s="7">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>260</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>265</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="G16" s="7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1563,20 +1585,20 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
@@ -1584,20 +1606,22 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="G18" s="3">
-        <v>51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -1605,20 +1629,20 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>62</v>
+        <v>30</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="3">
-        <v>54</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
@@ -1626,20 +1650,22 @@
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="3">
         <v>47</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="3">
-        <v>53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
@@ -1647,20 +1673,20 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="3">
-        <v>52</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1668,20 +1694,20 @@
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -1689,22 +1715,20 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="3">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -1712,20 +1736,20 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="3">
-        <v>49</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -1733,22 +1757,20 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="3">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -1756,125 +1778,125 @@
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="3">
-        <v>48</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="3">
-        <v>44</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="3">
-        <v>110</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="3">
-        <v>42</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="3">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>173</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="3">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -1882,20 +1904,20 @@
         <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="3">
-        <v>116</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -1903,20 +1925,20 @@
         <v>42</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="3">
-        <v>117</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
@@ -1924,20 +1946,20 @@
         <v>42</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="3">
-        <v>118</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
@@ -1945,20 +1967,20 @@
         <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>168</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="3">
-        <v>119</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1966,20 +1988,20 @@
         <v>42</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="3">
-        <v>120</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
@@ -1987,20 +2009,20 @@
         <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="3">
-        <v>112</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
@@ -2008,20 +2030,20 @@
         <v>42</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="3">
-        <v>114</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
@@ -2029,20 +2051,20 @@
         <v>42</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="3">
-        <v>115</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
@@ -2050,20 +2072,20 @@
         <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="3">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -2071,20 +2093,20 @@
         <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3">
-        <v>85</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -2092,20 +2114,20 @@
         <v>42</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="3">
-        <v>34</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
@@ -2113,20 +2135,20 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
@@ -2134,20 +2156,20 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="3">
-        <v>84</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -2155,20 +2177,20 @@
         <v>42</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="3">
-        <v>86</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
@@ -2176,20 +2198,20 @@
         <v>42</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -2197,20 +2219,20 @@
         <v>42</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="3">
-        <v>38</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -2218,20 +2240,20 @@
         <v>42</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="3">
-        <v>39</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -2239,20 +2261,20 @@
         <v>42</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -2260,20 +2282,20 @@
         <v>42</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
@@ -2281,20 +2303,20 @@
         <v>42</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="3">
-        <v>91</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -2302,20 +2324,20 @@
         <v>42</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="3">
-        <v>99</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -2323,20 +2345,20 @@
         <v>42</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="3">
-        <v>121</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -2344,20 +2366,20 @@
         <v>42</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -2365,20 +2387,20 @@
         <v>42</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
@@ -2386,20 +2408,20 @@
         <v>42</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="3">
-        <v>41</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -2407,20 +2429,20 @@
         <v>42</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>53</v>
       </c>
@@ -2428,20 +2450,20 @@
         <v>42</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="3">
-        <v>26</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
@@ -2449,20 +2471,20 @@
         <v>42</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="3">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
@@ -2470,20 +2492,20 @@
         <v>42</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="3">
-        <v>28</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>53</v>
       </c>
@@ -2491,20 +2513,20 @@
         <v>42</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>53</v>
       </c>
@@ -2512,20 +2534,20 @@
         <v>42</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="3">
-        <v>87</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>53</v>
       </c>
@@ -2533,20 +2555,20 @@
         <v>42</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="3">
-        <v>88</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>53</v>
       </c>
@@ -2554,20 +2576,20 @@
         <v>42</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="3">
-        <v>89</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
@@ -2575,20 +2597,20 @@
         <v>42</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="3">
-        <v>90</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>53</v>
       </c>
@@ -2596,20 +2618,20 @@
         <v>42</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="3">
-        <v>96</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>53</v>
       </c>
@@ -2617,20 +2639,20 @@
         <v>42</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="3">
-        <v>97</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>53</v>
       </c>
@@ -2638,20 +2660,20 @@
         <v>42</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="3">
-        <v>92</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>53</v>
       </c>
@@ -2659,20 +2681,20 @@
         <v>42</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="3">
-        <v>93</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>53</v>
       </c>
@@ -2680,20 +2702,20 @@
         <v>42</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>174</v>
+        <v>66</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="3">
-        <v>94</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>53</v>
       </c>
@@ -2701,20 +2723,20 @@
         <v>42</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>178</v>
+        <v>110</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>174</v>
+        <v>111</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>53</v>
       </c>
@@ -2722,20 +2744,20 @@
         <v>42</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>53</v>
       </c>
@@ -2743,20 +2765,20 @@
         <v>42</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>183</v>
+        <v>109</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>53</v>
       </c>
@@ -2764,20 +2786,20 @@
         <v>42</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>53</v>
       </c>
@@ -2785,20 +2807,20 @@
         <v>42</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>53</v>
       </c>
@@ -2806,20 +2828,20 @@
         <v>42</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>53</v>
       </c>
@@ -2827,20 +2849,20 @@
         <v>42</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>53</v>
       </c>
@@ -2848,20 +2870,20 @@
         <v>42</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="3">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>53</v>
       </c>
@@ -2869,765 +2891,808 @@
         <v>42</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>53</v>
+        <v>197</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>197</v>
+        <v>255</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>126</v>
+        <v>256</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>53</v>
+        <v>197</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>198</v>
+        <v>250</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F81" s="1"/>
+        <v>251</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="G81" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>201</v>
+        <v>238</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="3">
-        <v>81</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>204</v>
+        <v>258</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>206</v>
+        <v>188</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="3">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>209</v>
+        <v>128</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="3">
-        <v>79</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>210</v>
+        <v>244</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>212</v>
+        <v>245</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="3">
-        <v>83</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="3">
-        <v>76</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>216</v>
+        <v>257</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>102</v>
+        <v>186</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F87" s="1"/>
+      <c r="G87" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F88" s="1"/>
+      <c r="G88" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G87" s="3">
-        <v>111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G88" s="3">
-        <v>113</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
-      <c r="A89" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="D89" s="1" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="3">
-        <v>78</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>224</v>
+        <v>66</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="3">
-        <v>67</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="3">
-        <v>63</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>128</v>
+        <v>190</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="3">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="3">
-        <v>66</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>230</v>
+        <v>102</v>
       </c>
       <c r="E95" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G95" s="3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G96" s="3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F97" s="1"/>
+      <c r="G97" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F95" s="1"/>
-      <c r="G95" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
-      <c r="A96" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F96" s="1"/>
-      <c r="G96" s="3">
-        <v>102</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F97" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="G97" s="3">
-        <v>104</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="3">
-        <v>77</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>240</v>
+        <v>58</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="3">
-        <v>69</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="3">
-        <v>105</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>61</v>
+        <v>221</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G103" s="3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F104" s="1"/>
+      <c r="G104" s="3">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
-      <c r="A103" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F103" s="1"/>
-      <c r="G103" s="3">
-        <v>59</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
-      <c r="A104" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G104" s="3">
-        <v>72</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+    <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>151</v>
+        <v>231</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="3">
-        <v>68</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>240</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>241</v>
+      </c>
       <c r="G106" s="3">
-        <v>64</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>254</v>
+        <v>44</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="3">
-        <v>73</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>255</v>
+        <v>38</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F108" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G108" s="3">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>200</v>
+        <v>53</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>256</v>
+        <v>82</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>257</v>
+        <v>83</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>258</v>
+        <v>40</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="3">
-        <v>71</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>200</v>
+        <v>53</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>259</v>
+        <v>79</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>260</v>
+        <v>80</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>262</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F110" s="1"/>
       <c r="G110" s="3">
-        <v>103</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>200</v>
+        <v>53</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>263</v>
+        <v>87</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>264</v>
+        <v>88</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>265</v>
+        <v>89</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
-      <c r="A112" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G112" s="8">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G113" s="8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G114" s="8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E115" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F112" s="1"/>
-      <c r="G112" s="3">
-        <v>58</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
-      <c r="A113" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F113" s="1"/>
-      <c r="G113" s="3">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
-      <c r="A114" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F114" s="1"/>
-      <c r="G114" s="3">
-        <v>57</v>
+      <c r="G115" s="8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G116" s="8">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:G116">
+    <sortCondition ref="B2:B116" customList="file structure,dq,pdde"/>
+    <sortCondition ref="A2:A116" customList="High Priority,Error,Warning"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-ordered columns so source is first, since that's how we're sorting
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\rstudio-export (10)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SilvermanA\eva\public-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="EvaChecks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">EvaChecks!$A$1:$G$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">EvaChecks!$B$1:$G$111</definedName>
   </definedNames>
   <calcPr calcId="4264353701"/>
 </workbook>
@@ -1220,7 +1220,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,10 +1235,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1258,10 +1258,10 @@
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -1321,10 +1321,10 @@
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>29</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>26</v>
@@ -1388,10 +1388,10 @@
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>263</v>
@@ -1409,10 +1409,10 @@
     </row>
     <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -1430,10 +1430,10 @@
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
@@ -1453,10 +1453,10 @@
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>261</v>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>264</v>
@@ -1537,10 +1537,10 @@
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>262</v>
@@ -1558,10 +1558,10 @@
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>260</v>
@@ -1579,10 +1579,10 @@
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>72</v>
@@ -1600,10 +1600,10 @@
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>29</v>
@@ -1623,10 +1623,10 @@
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>26</v>
@@ -1667,10 +1667,10 @@
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>68</v>
@@ -1688,10 +1688,10 @@
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>60</v>
@@ -1709,10 +1709,10 @@
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>57</v>
@@ -1730,10 +1730,10 @@
     </row>
     <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>65</v>
@@ -1751,10 +1751,10 @@
     </row>
     <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>63</v>
@@ -1772,10 +1772,10 @@
     </row>
     <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>54</v>
@@ -1793,10 +1793,10 @@
     </row>
     <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>43</v>
@@ -1814,10 +1814,10 @@
     </row>
     <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>51</v>
@@ -1835,10 +1835,10 @@
     </row>
     <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>46</v>
@@ -1856,10 +1856,10 @@
     </row>
     <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>49</v>
@@ -1877,10 +1877,10 @@
     </row>
     <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>173</v>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>175</v>
@@ -1919,10 +1919,10 @@
     </row>
     <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>161</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>165</v>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>168</v>
@@ -1982,10 +1982,10 @@
     </row>
     <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>90</v>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>95</v>
@@ -2024,10 +2024,10 @@
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>97</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>99</v>
@@ -2066,10 +2066,10 @@
     </row>
     <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>93</v>
@@ -2087,10 +2087,10 @@
     </row>
     <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>104</v>
@@ -2108,10 +2108,10 @@
     </row>
     <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>101</v>
@@ -2129,10 +2129,10 @@
     </row>
     <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>106</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>133</v>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>170</v>
@@ -2192,10 +2192,10 @@
     </row>
     <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>172</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>159</v>
@@ -2234,10 +2234,10 @@
     </row>
     <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>163</v>
@@ -2255,10 +2255,10 @@
     </row>
     <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>147</v>
@@ -2276,10 +2276,10 @@
     </row>
     <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>118</v>
@@ -2297,10 +2297,10 @@
     </row>
     <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>179</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>183</v>
@@ -2339,10 +2339,10 @@
     </row>
     <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>144</v>
@@ -2360,10 +2360,10 @@
     </row>
     <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>155</v>
@@ -2381,10 +2381,10 @@
     </row>
     <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>139</v>
@@ -2402,10 +2402,10 @@
     </row>
     <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>131</v>
@@ -2423,10 +2423,10 @@
     </row>
     <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>187</v>
@@ -2444,10 +2444,10 @@
     </row>
     <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>113</v>
@@ -2465,10 +2465,10 @@
     </row>
     <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>116</v>
@@ -2486,10 +2486,10 @@
     </row>
     <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>142</v>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>127</v>
@@ -2528,10 +2528,10 @@
     </row>
     <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>195</v>
@@ -2549,10 +2549,10 @@
     </row>
     <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>151</v>
@@ -2570,10 +2570,10 @@
     </row>
     <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>185</v>
@@ -2591,10 +2591,10 @@
     </row>
     <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>157</v>
@@ -2612,10 +2612,10 @@
     </row>
     <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>108</v>
@@ -2633,10 +2633,10 @@
     </row>
     <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>191</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>153</v>
@@ -2675,10 +2675,10 @@
     </row>
     <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>124</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>150</v>
@@ -2717,10 +2717,10 @@
     </row>
     <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>110</v>
@@ -2738,10 +2738,10 @@
     </row>
     <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>193</v>
@@ -2759,10 +2759,10 @@
     </row>
     <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>129</v>
@@ -2780,10 +2780,10 @@
     </row>
     <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>189</v>
@@ -2801,10 +2801,10 @@
     </row>
     <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>177</v>
@@ -2822,10 +2822,10 @@
     </row>
     <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>181</v>
@@ -2843,10 +2843,10 @@
     </row>
     <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>166</v>
@@ -2864,10 +2864,10 @@
     </row>
     <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>121</v>
@@ -2885,10 +2885,10 @@
     </row>
     <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>136</v>
@@ -2906,10 +2906,10 @@
     </row>
     <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>254</v>
@@ -2927,10 +2927,10 @@
     </row>
     <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>250</v>
@@ -2950,10 +2950,10 @@
     </row>
     <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>238</v>
@@ -2971,10 +2971,10 @@
     </row>
     <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>258</v>
@@ -2992,10 +2992,10 @@
     </row>
     <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>218</v>
@@ -3013,10 +3013,10 @@
     </row>
     <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>244</v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>242</v>
@@ -3055,10 +3055,10 @@
     </row>
     <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>257</v>
@@ -3076,10 +3076,10 @@
     </row>
     <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>246</v>
@@ -3097,10 +3097,10 @@
     </row>
     <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>217</v>
@@ -3118,10 +3118,10 @@
     </row>
     <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>243</v>
@@ -3139,10 +3139,10 @@
     </row>
     <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>214</v>
@@ -3160,10 +3160,10 @@
     </row>
     <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>219</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>259</v>
@@ -3202,10 +3202,10 @@
     </row>
     <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>216</v>
@@ -3223,10 +3223,10 @@
     </row>
     <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>207</v>
@@ -3246,10 +3246,10 @@
     </row>
     <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>210</v>
@@ -3269,10 +3269,10 @@
     </row>
     <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>220</v>
@@ -3290,10 +3290,10 @@
     </row>
     <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>235</v>
@@ -3311,10 +3311,10 @@
     </row>
     <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>233</v>
@@ -3332,10 +3332,10 @@
     </row>
     <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>212</v>
@@ -3353,10 +3353,10 @@
     </row>
     <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>247</v>
@@ -3374,10 +3374,10 @@
     </row>
     <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>223</v>
@@ -3395,10 +3395,10 @@
     </row>
     <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>225</v>
@@ -3418,10 +3418,10 @@
     </row>
     <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>237</v>
@@ -3439,10 +3439,10 @@
     </row>
     <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>230</v>
@@ -3460,10 +3460,10 @@
     </row>
     <row r="106" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>239</v>
@@ -3483,10 +3483,10 @@
     </row>
     <row r="107" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>228</v>
@@ -3504,10 +3504,10 @@
     </row>
     <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>38</v>
@@ -3527,10 +3527,10 @@
     </row>
     <row r="109" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>82</v>
@@ -3548,10 +3548,10 @@
     </row>
     <row r="110" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>79</v>
@@ -3569,10 +3569,10 @@
     </row>
     <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>87</v>
@@ -3590,10 +3590,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>76</v>
@@ -3610,10 +3610,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>84</v>
@@ -3630,10 +3630,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B114" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>201</v>
@@ -3650,10 +3650,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>198</v>
@@ -3670,10 +3670,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>204</v>
@@ -3689,9 +3689,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G116">
-    <sortCondition ref="B2:B116" customList="file structure,dq,pdde"/>
-    <sortCondition ref="A2:A116" customList="High Priority,Error,Warning"/>
+  <sortState ref="B2:H116">
+    <sortCondition ref="B2:B116" customList="High Priority,Error,Warning"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added zip extension check to EvaChecks and updated initially_valid_import script to pull "issue" and "guidance" from EvaChecks, rather than hardcoding.
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -15,14 +15,14 @@
     <sheet name="EvaChecks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">EvaChecks!$B$1:$G$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EvaChecks!$A$1:$G$117</definedName>
   </definedNames>
   <calcPr calcId="4264353701"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="275">
   <si>
     <t>Type</t>
   </si>
@@ -841,6 +841,12 @@
   </si>
   <si>
     <t>Your zip file appears to be missing the following files: [files listed] You either uploaded something other than an HMIS CSV export or your export does not contain all the files outlined in the HMIS CSV Export specifications. If you are not sure how to run the hashed HMIS CSV Export in your HMIS, please contact your HMIS vendor.</t>
+  </si>
+  <si>
+    <t>Wrong File Type</t>
+  </si>
+  <si>
+    <t>Eva can only import .zip files. If you are using a 7-zip file, please contact your vendor for help converting to the .zip format.</t>
   </si>
 </sst>
 </file>
@@ -1216,11 +1222,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C5"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,24 +1500,23 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="7">
-        <v>123</v>
+      <c r="E13" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G13" s="3">
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1522,17 +1527,17 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="7">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1543,17 +1548,17 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="7">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1564,17 +1569,17 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="7">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1582,20 +1587,20 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>72</v>
+        <v>260</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>265</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="3">
-        <v>49</v>
+      <c r="G17" s="7">
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1606,19 +1611,17 @@
         <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="3">
-        <v>82</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1629,17 +1632,19 @@
         <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="G19" s="3">
-        <v>48</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1650,19 +1655,17 @@
         <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1673,17 +1676,19 @@
         <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="G21" s="3">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1694,17 +1699,17 @@
         <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1715,17 +1720,17 @@
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="3">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1736,17 +1741,17 @@
         <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="3">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1757,17 +1762,17 @@
         <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="3">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1778,38 +1783,38 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="3">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1820,17 +1825,17 @@
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1841,17 +1846,17 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1862,17 +1867,17 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1880,20 +1885,20 @@
         <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>173</v>
+        <v>49</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>171</v>
+        <v>47</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>174</v>
+        <v>50</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="3">
-        <v>94</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1904,17 +1909,17 @@
         <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>171</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="3">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1925,17 +1930,17 @@
         <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="3">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1946,7 +1951,7 @@
         <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>160</v>
@@ -1956,7 +1961,7 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="3">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1967,17 +1972,17 @@
         <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="3">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1988,17 +1993,17 @@
         <v>53</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>90</v>
+        <v>168</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="3">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2009,17 +2014,17 @@
         <v>53</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="3">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2030,17 +2035,17 @@
         <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="3">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,17 +2056,17 @@
         <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="3">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2072,17 +2077,17 @@
         <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="3">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,17 +2098,17 @@
         <v>53</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="3">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2114,17 +2119,17 @@
         <v>53</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="3">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2135,17 +2140,17 @@
         <v>53</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="3">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2156,17 +2161,17 @@
         <v>53</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="3">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2177,17 +2182,17 @@
         <v>53</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="3">
-        <v>92</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2198,17 +2203,17 @@
         <v>53</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>171</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2219,17 +2224,17 @@
         <v>53</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="3">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2240,17 +2245,17 @@
         <v>53</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="3">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2261,17 +2266,17 @@
         <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="3">
-        <v>41</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2282,17 +2287,17 @@
         <v>53</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="3">
-        <v>84</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2303,17 +2308,17 @@
         <v>53</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>179</v>
+        <v>118</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="3">
-        <v>16</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2324,17 +2329,17 @@
         <v>53</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2345,17 +2350,17 @@
         <v>53</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="3">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2366,17 +2371,17 @@
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="3">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2387,17 +2392,17 @@
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="3">
-        <v>121</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2408,17 +2413,17 @@
         <v>53</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="3">
-        <v>32</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2429,17 +2434,17 @@
         <v>53</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="3">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2450,17 +2455,17 @@
         <v>53</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="3">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2471,17 +2476,17 @@
         <v>53</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>115</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="3">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2492,17 +2497,17 @@
         <v>53</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="3">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,17 +2518,17 @@
         <v>53</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="3">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2534,17 +2539,17 @@
         <v>53</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>195</v>
+        <v>127</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="3">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2555,17 +2560,17 @@
         <v>53</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2576,17 +2581,17 @@
         <v>53</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="3">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2597,17 +2602,17 @@
         <v>53</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="3">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2618,17 +2623,17 @@
         <v>53</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="3">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2639,17 +2644,17 @@
         <v>53</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>191</v>
+        <v>108</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>192</v>
+        <v>58</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="3">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2660,17 +2665,17 @@
         <v>53</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="3">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2681,17 +2686,17 @@
         <v>53</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="3">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2702,17 +2707,17 @@
         <v>53</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2723,17 +2728,17 @@
         <v>53</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="3">
-        <v>85</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2744,17 +2749,17 @@
         <v>53</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>193</v>
+        <v>110</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="3">
-        <v>23</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2765,17 +2770,17 @@
         <v>53</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>129</v>
+        <v>193</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>130</v>
+        <v>194</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="3">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2786,17 +2791,17 @@
         <v>53</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="3">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2807,17 +2812,17 @@
         <v>53</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="3">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2828,17 +2833,17 @@
         <v>53</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2849,17 +2854,17 @@
         <v>53</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="3">
-        <v>96</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2870,17 +2875,17 @@
         <v>53</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="3">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2891,17 +2896,17 @@
         <v>53</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="3">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2909,20 +2914,20 @@
         <v>42</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>197</v>
+        <v>53</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>254</v>
+        <v>136</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>255</v>
+        <v>137</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>256</v>
+        <v>138</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="3">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2933,19 +2938,17 @@
         <v>197</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>253</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F81" s="1"/>
       <c r="G81" s="3">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2956,17 +2959,19 @@
         <v>197</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F82" s="1"/>
+        <v>251</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="G82" s="3">
-        <v>59</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2977,17 +2982,17 @@
         <v>197</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E83" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="3">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2998,17 +3003,17 @@
         <v>197</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>218</v>
+        <v>258</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>213</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="3">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3019,17 +3024,17 @@
         <v>197</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>245</v>
+        <v>128</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>213</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="3">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3040,17 +3045,17 @@
         <v>197</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E86" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E86" s="4" t="s">
         <v>213</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="3">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3061,17 +3066,17 @@
         <v>197</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="3">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3082,17 +3087,17 @@
         <v>197</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="3">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3103,17 +3108,17 @@
         <v>197</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="3">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3124,17 +3129,17 @@
         <v>197</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="3">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3145,17 +3150,17 @@
         <v>197</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>215</v>
+        <v>66</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3166,17 +3171,17 @@
         <v>197</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="3">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3187,17 +3192,17 @@
         <v>197</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="3">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3208,17 +3213,17 @@
         <v>197</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>216</v>
+        <v>259</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>114</v>
+        <v>190</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>213</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="3">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3229,19 +3234,17 @@
         <v>197</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>209</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="F95" s="1"/>
       <c r="G95" s="3">
-        <v>111</v>
+        <v>60</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3252,19 +3255,19 @@
         <v>197</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>209</v>
       </c>
       <c r="G96" s="3">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3275,17 +3278,19 @@
         <v>197</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>221</v>
+        <v>102</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F97" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G97" s="3">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3296,17 +3301,17 @@
         <v>197</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="3">
-        <v>105</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3317,17 +3322,17 @@
         <v>197</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>231</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="3">
-        <v>69</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3338,17 +3343,17 @@
         <v>197</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>58</v>
+        <v>231</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="3">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3359,17 +3364,17 @@
         <v>197</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>248</v>
+        <v>58</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="3">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3380,17 +3385,17 @@
         <v>197</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="3">
-        <v>102</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3401,19 +3406,17 @@
         <v>197</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>221</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>227</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="F103" s="1"/>
       <c r="G103" s="3">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3424,17 +3427,19 @@
         <v>197</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>61</v>
+        <v>221</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F104" s="1"/>
+        <v>226</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="G104" s="3">
-        <v>74</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3445,17 +3450,17 @@
         <v>197</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>231</v>
+        <v>61</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="3">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3466,19 +3471,17 @@
         <v>197</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>241</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="F106" s="1"/>
       <c r="G106" s="3">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3489,40 +3492,40 @@
         <v>197</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F107" s="1"/>
+        <v>240</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>241</v>
+      </c>
       <c r="G107" s="3">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>38</v>
+        <v>228</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="F108" s="1"/>
       <c r="G108" s="3">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3530,20 +3533,22 @@
         <v>37</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F109" s="1"/>
+      <c r="F109" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G109" s="3">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3554,17 +3559,17 @@
         <v>53</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="3">
-        <v>110</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3575,37 +3580,38 @@
         <v>53</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F112" s="1"/>
+      <c r="G112" s="3">
         <v>43</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E112" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G112" s="8">
-        <v>44</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3616,16 +3622,16 @@
         <v>53</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G113" s="8">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3633,19 +3639,19 @@
         <v>37</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>197</v>
+        <v>53</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>201</v>
+        <v>84</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>202</v>
+        <v>85</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>203</v>
+        <v>86</v>
       </c>
       <c r="G114" s="8">
-        <v>79</v>
+        <v>46</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3656,16 +3662,16 @@
         <v>197</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G115" s="8">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3676,19 +3682,40 @@
         <v>197</v>
       </c>
       <c r="C116" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G116" s="8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C117" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D117" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E116" s="4" t="s">
+      <c r="E117" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="G116" s="8">
+      <c r="G117" s="8">
         <v>83</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G117"/>
   <sortState ref="B2:H116">
     <sortCondition ref="B2:B116" customList="High Priority,Error,Warning"/>
   </sortState>

</xml_diff>

<commit_message>
added 2 new issues to the evachecks
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="EvaChecks" sheetId="1" r:id="rId1"/>
+    <sheet name="EvaChecks (11)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EvaChecks!$A$1:$G$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EvaChecks (11)'!$A$1:$G$119</definedName>
   </definedNames>
   <calcPr calcId="4264353701"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="281">
   <si>
     <t>Type</t>
   </si>
@@ -847,6 +847,24 @@
   </si>
   <si>
     <t>Residential projects should have inventory data. Please enter inventory in HMIS for the project.</t>
+  </si>
+  <si>
+    <t>Overlapping CE Participation Records</t>
+  </si>
+  <si>
+    <t>This project has more than one CE Participation record that covers the same time period. Please be sure you are ending any records that are no longer accurate before creating a new record.</t>
+  </si>
+  <si>
+    <t>2.09 CE Participation Status</t>
+  </si>
+  <si>
+    <t>Overlapping HMIS Participation Records</t>
+  </si>
+  <si>
+    <t>2.08 HMIS Participation</t>
+  </si>
+  <si>
+    <t>This project has more than one HMIS Participation record that covers the same time period. Please be sure you are ending any records that are no longer accurate before creating a new record.</t>
   </si>
 </sst>
 </file>
@@ -1228,11 +1246,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3557,46 +3575,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F110" s="1"/>
-      <c r="G110" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="B110" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G110" s="4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F111" s="1"/>
-      <c r="G111" s="2">
-        <v>110</v>
+      <c r="B111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G111" s="4">
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3607,57 +3623,59 @@
         <v>53</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>274</v>
+        <v>40</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F113" s="1"/>
+      <c r="G113" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F114" s="1"/>
+      <c r="G114" s="2">
         <v>43</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G113" s="7">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G114" s="7">
-        <v>46</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3665,19 +3683,19 @@
         <v>37</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>196</v>
+        <v>53</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>200</v>
+        <v>76</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>201</v>
+        <v>77</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>202</v>
+        <v>78</v>
       </c>
       <c r="G115" s="7">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3685,19 +3703,19 @@
         <v>37</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>196</v>
+        <v>53</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>197</v>
+        <v>84</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>198</v>
+        <v>85</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="G116" s="7">
-        <v>81</v>
+        <v>46</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3708,20 +3726,60 @@
         <v>196</v>
       </c>
       <c r="C117" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G117" s="7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G118" s="7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D119" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E119" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G117" s="7">
+      <c r="G119" s="7">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G117"/>
+  <autoFilter ref="A1:G119"/>
   <sortState ref="B2:H116">
     <sortCondition ref="B2:B116" customList="High Priority,Error,Warning"/>
   </sortState>

</xml_diff>

<commit_message>
added new pdde check for RRH SOs with active inventory records
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F1A671-C679-4C30-BEC3-5B121197A916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EvaChecks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EvaChecks!$A$1:$G$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EvaChecks!$A$1:$G$118</definedName>
   </definedNames>
   <calcPr calcId="4264353701"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="278">
   <si>
     <t>Type</t>
   </si>
@@ -847,12 +848,21 @@
   </si>
   <si>
     <t>Residential projects should have inventory data. Please enter inventory in HMIS for the project.</t>
+  </si>
+  <si>
+    <t>RRH-SO has active bed inventory</t>
+  </si>
+  <si>
+    <t>2.02.6 ProjectType, 2.02.A RRHSubType, 2.07.14 Bed Inventory, 2.07 Inventory Start and End Dates</t>
+  </si>
+  <si>
+    <t>You have designated this project as Rapid Rehousing, subtype Services Only. The FY2024 Data Standards Manual says this kind of project "provides services only and does not provide ongoing rental assistance or support any inventory for participants." If the project fits this description, please be sure there are no active inventory records associated with the project.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,13 +911,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -917,7 +925,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1224,2506 +1232,2427 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18" style="3" customWidth="1"/>
-    <col min="5" max="5" width="32" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>264</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>272</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>264</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>273</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>260</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>264</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>268</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="6">
+      <c r="G14" s="4">
         <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>263</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>266</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="6">
+      <c r="G15" s="4">
         <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>261</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>265</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="6">
+      <c r="G16" s="4">
         <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>259</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>264</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="6">
+      <c r="G17" s="4">
         <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
         <v>172</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>173</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>170</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>175</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="2">
+      <c r="G33" s="1">
         <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>159</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>161</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
         <v>164</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>161</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="2">
+      <c r="G35" s="1">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
         <v>167</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>166</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>168</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="2">
+      <c r="G36" s="1">
         <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>91</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="2">
+      <c r="G37" s="1">
         <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>95</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="2">
+      <c r="G38" s="1">
         <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
         <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>90</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="2">
+      <c r="G40" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>93</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>101</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
         <v>100</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>101</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>102</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
         <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>106</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="2">
+      <c r="G44" s="1">
         <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>134</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
         <v>169</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>170</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>125</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="2">
+      <c r="G46" s="1">
         <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="s">
         <v>171</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>170</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>163</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="2">
+      <c r="G47" s="1">
         <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>159</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>125</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="2">
+      <c r="G48" s="1">
         <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="A49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" t="s">
         <v>162</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>159</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>163</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="2">
+      <c r="G49" s="1">
         <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="A50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" t="s">
         <v>146</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>147</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>148</v>
       </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="2">
+      <c r="G50" s="1">
         <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>118</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>119</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="2">
+      <c r="G51" s="1">
         <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
         <v>178</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>177</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>179</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="2">
+      <c r="G52" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" t="s">
         <v>182</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>181</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>183</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="2">
+      <c r="G53" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="A54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" t="s">
         <v>143</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>144</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>145</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="2">
+      <c r="G54" s="1">
         <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" t="s">
         <v>154</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>155</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>125</v>
       </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="2">
+      <c r="G55" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>140</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="2">
+      <c r="G56" s="1">
         <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" t="s">
         <v>130</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>125</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="2">
+      <c r="G57" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" t="s">
         <v>186</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>187</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>125</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="2">
+      <c r="G58" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="A59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>113</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>114</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="2">
+      <c r="G59" s="1">
         <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>114</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="2">
+      <c r="G60" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" t="s">
         <v>141</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>142</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>125</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="2">
+      <c r="G61" s="1">
         <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" t="s">
+        <v>53</v>
+      </c>
+      <c r="C62" t="s">
         <v>126</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" t="s">
         <v>127</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>125</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="2">
+      <c r="G62" s="1">
         <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" t="s">
         <v>194</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" t="s">
         <v>195</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>125</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="2">
+      <c r="G63" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" t="s">
+        <v>53</v>
+      </c>
+      <c r="C64" t="s">
         <v>150</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>151</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>125</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="2">
+      <c r="G64" s="1">
         <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" t="s">
         <v>184</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>185</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>125</v>
       </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="2">
+      <c r="G65" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" t="s">
         <v>156</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>157</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>125</v>
       </c>
-      <c r="F66" s="1"/>
-      <c r="G66" s="2">
+      <c r="G66" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="A67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" t="s">
+        <v>53</v>
+      </c>
+      <c r="C67" t="s">
         <v>107</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>58</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>108</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="2">
+      <c r="G67" s="1">
         <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="A68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68" t="s">
         <v>190</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>191</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>125</v>
       </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="2">
+      <c r="G68" s="1">
         <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" t="s">
         <v>152</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>153</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>125</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="2">
+      <c r="G69" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" t="s">
         <v>123</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" t="s">
         <v>124</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="2">
+      <c r="G70" s="1">
         <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" t="s">
         <v>149</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>66</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>125</v>
       </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="2">
+      <c r="G71" s="1">
         <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C72" s="1" t="s">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C72" t="s">
         <v>109</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>110</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>111</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="2">
+      <c r="G72" s="1">
         <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C73" s="1" t="s">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" t="s">
         <v>192</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>193</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" t="s">
         <v>125</v>
       </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="2">
+      <c r="G73" s="1">
         <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74" t="s">
         <v>128</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>129</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" t="s">
         <v>108</v>
       </c>
-      <c r="F74" s="1"/>
-      <c r="G74" s="2">
+      <c r="G74" s="1">
         <v>39</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="A75" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" t="s">
         <v>188</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>189</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" t="s">
         <v>125</v>
       </c>
-      <c r="F75" s="1"/>
-      <c r="G75" s="2">
+      <c r="G75" s="1">
         <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C76" s="1" t="s">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" t="s">
+        <v>53</v>
+      </c>
+      <c r="C76" t="s">
         <v>176</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>177</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>125</v>
       </c>
-      <c r="F76" s="1"/>
-      <c r="G76" s="2">
+      <c r="G76" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C77" s="1" t="s">
+      <c r="A77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" t="s">
         <v>181</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>125</v>
       </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="2">
+      <c r="G77" s="1">
         <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="A78" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" t="s">
         <v>165</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" t="s">
         <v>166</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" t="s">
         <v>125</v>
       </c>
-      <c r="F78" s="1"/>
-      <c r="G78" s="2">
+      <c r="G78" s="1">
         <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="A79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" t="s">
         <v>120</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" t="s">
         <v>121</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" t="s">
         <v>122</v>
       </c>
-      <c r="F79" s="1"/>
-      <c r="G79" s="2">
+      <c r="G79" s="1">
         <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="A80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" t="s">
         <v>135</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" t="s">
         <v>136</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" t="s">
         <v>137</v>
       </c>
-      <c r="F80" s="1"/>
-      <c r="G80" s="2">
+      <c r="G80" s="1">
         <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B81" s="1" t="s">
+      <c r="A81" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" t="s">
         <v>196</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" t="s">
         <v>253</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" t="s">
         <v>254</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" t="s">
         <v>255</v>
       </c>
-      <c r="F81" s="1"/>
-      <c r="G81" s="2">
+      <c r="G81" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B82" s="1" t="s">
+      <c r="A82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" t="s">
         <v>196</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" t="s">
         <v>249</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" t="s">
         <v>250</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E82" t="s">
         <v>251</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F82" t="s">
         <v>252</v>
       </c>
-      <c r="G82" s="2">
+      <c r="G82" s="1">
         <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B83" s="1" t="s">
+      <c r="A83" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" t="s">
         <v>237</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" t="s">
         <v>61</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" t="s">
         <v>212</v>
       </c>
-      <c r="F83" s="1"/>
-      <c r="G83" s="2">
+      <c r="G83" s="1">
         <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B84" s="1" t="s">
+      <c r="A84" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" t="s">
         <v>196</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" t="s">
         <v>257</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" t="s">
         <v>187</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E84" t="s">
         <v>212</v>
       </c>
-      <c r="F84" s="1"/>
-      <c r="G84" s="2">
+      <c r="G84" s="1">
         <v>56</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B85" s="1" t="s">
+      <c r="A85" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" t="s">
         <v>196</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" t="s">
         <v>217</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" t="s">
         <v>127</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E85" t="s">
         <v>212</v>
       </c>
-      <c r="F85" s="1"/>
-      <c r="G85" s="2">
+      <c r="G85" s="1">
         <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B86" s="1" t="s">
+      <c r="A86" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" t="s">
         <v>196</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>243</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" t="s">
         <v>244</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E86" t="s">
         <v>212</v>
       </c>
-      <c r="F86" s="1"/>
-      <c r="G86" s="2">
+      <c r="G86" s="1">
         <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B87" s="1" t="s">
+      <c r="A87" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" t="s">
         <v>196</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>241</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" t="s">
         <v>147</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E87" t="s">
         <v>212</v>
       </c>
-      <c r="F87" s="1"/>
-      <c r="G87" s="2">
+      <c r="G87" s="1">
         <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B88" s="1" t="s">
+      <c r="A88" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" t="s">
         <v>196</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" t="s">
         <v>256</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" t="s">
         <v>185</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>212</v>
       </c>
-      <c r="F88" s="1"/>
-      <c r="G88" s="2">
+      <c r="G88" s="1">
         <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B89" s="1" t="s">
+      <c r="A89" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" t="s">
         <v>196</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" t="s">
         <v>245</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" t="s">
         <v>157</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" t="s">
         <v>212</v>
       </c>
-      <c r="F89" s="1"/>
-      <c r="G89" s="2">
+      <c r="G89" s="1">
         <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B90" s="1" t="s">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" t="s">
         <v>196</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" t="s">
         <v>216</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" t="s">
         <v>124</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>212</v>
       </c>
-      <c r="F90" s="1"/>
-      <c r="G90" s="2">
+      <c r="G90" s="1">
         <v>63</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B91" s="1" t="s">
+      <c r="A91" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" t="s">
         <v>196</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" t="s">
         <v>242</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" t="s">
         <v>66</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" t="s">
         <v>212</v>
       </c>
-      <c r="F91" s="1"/>
-      <c r="G91" s="2">
+      <c r="G91" s="1">
         <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B92" s="1" t="s">
+      <c r="A92" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92" t="s">
         <v>196</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" t="s">
         <v>213</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" t="s">
         <v>214</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" t="s">
         <v>212</v>
       </c>
-      <c r="F92" s="1"/>
-      <c r="G92" s="2">
+      <c r="G92" s="1">
         <v>67</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B93" s="1" t="s">
+      <c r="A93" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" t="s">
         <v>196</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" t="s">
         <v>218</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" t="s">
         <v>129</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" t="s">
         <v>212</v>
       </c>
-      <c r="F93" s="1"/>
-      <c r="G93" s="2">
+      <c r="G93" s="1">
         <v>66</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B94" s="1" t="s">
+      <c r="A94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" t="s">
         <v>196</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" t="s">
         <v>258</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" t="s">
         <v>189</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E94" t="s">
         <v>212</v>
       </c>
-      <c r="F94" s="1"/>
-      <c r="G94" s="2">
+      <c r="G94" s="1">
         <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B95" s="1" t="s">
+      <c r="A95" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" t="s">
         <v>196</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" t="s">
         <v>215</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" t="s">
         <v>113</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="E95" t="s">
         <v>212</v>
       </c>
-      <c r="F95" s="1"/>
-      <c r="G95" s="2">
+      <c r="G95" s="1">
         <v>60</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B96" s="1" t="s">
+      <c r="A96" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" t="s">
         <v>196</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" t="s">
         <v>206</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" t="s">
         <v>101</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E96" t="s">
         <v>207</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F96" t="s">
         <v>208</v>
       </c>
-      <c r="G96" s="2">
+      <c r="G96" s="1">
         <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B97" s="1" t="s">
+      <c r="A97" t="s">
+        <v>42</v>
+      </c>
+      <c r="B97" t="s">
         <v>196</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" t="s">
         <v>209</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" t="s">
         <v>101</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="E97" t="s">
         <v>210</v>
       </c>
-      <c r="F97" s="1" t="s">
+      <c r="F97" t="s">
         <v>208</v>
       </c>
-      <c r="G97" s="2">
+      <c r="G97" s="1">
         <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B98" s="1" t="s">
+      <c r="A98" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" t="s">
         <v>219</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" t="s">
         <v>220</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E98" t="s">
         <v>221</v>
       </c>
-      <c r="F98" s="1"/>
-      <c r="G98" s="2">
+      <c r="G98" s="1">
         <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B99" s="1" t="s">
+      <c r="A99" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" t="s">
         <v>196</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" t="s">
         <v>234</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" t="s">
         <v>230</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E99" t="s">
         <v>235</v>
       </c>
-      <c r="F99" s="1"/>
-      <c r="G99" s="2">
+      <c r="G99" s="1">
         <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B100" s="1" t="s">
+      <c r="A100" t="s">
+        <v>42</v>
+      </c>
+      <c r="B100" t="s">
         <v>196</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" t="s">
         <v>232</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" t="s">
         <v>230</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E100" t="s">
         <v>233</v>
       </c>
-      <c r="F100" s="1"/>
-      <c r="G100" s="2">
+      <c r="G100" s="1">
         <v>69</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B101" s="1" t="s">
+      <c r="A101" t="s">
+        <v>42</v>
+      </c>
+      <c r="B101" t="s">
         <v>196</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" t="s">
         <v>211</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" t="s">
         <v>58</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" t="s">
         <v>212</v>
       </c>
-      <c r="F101" s="1"/>
-      <c r="G101" s="2">
+      <c r="G101" s="1">
         <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B102" s="1" t="s">
+      <c r="A102" t="s">
+        <v>42</v>
+      </c>
+      <c r="B102" t="s">
         <v>196</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" t="s">
         <v>246</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" t="s">
         <v>247</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E102" t="s">
         <v>248</v>
       </c>
-      <c r="F102" s="1"/>
-      <c r="G102" s="2">
+      <c r="G102" s="1">
         <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B103" s="1" t="s">
+      <c r="A103" t="s">
+        <v>42</v>
+      </c>
+      <c r="B103" t="s">
         <v>196</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" t="s">
         <v>222</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" t="s">
         <v>220</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E103" t="s">
         <v>223</v>
       </c>
-      <c r="F103" s="1"/>
-      <c r="G103" s="2">
+      <c r="G103" s="1">
         <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B104" s="1" t="s">
+      <c r="A104" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" t="s">
         <v>196</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" t="s">
         <v>224</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" t="s">
         <v>220</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E104" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F104" t="s">
         <v>226</v>
       </c>
-      <c r="G104" s="2">
+      <c r="G104" s="1">
         <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B105" s="1" t="s">
+      <c r="A105" t="s">
+        <v>42</v>
+      </c>
+      <c r="B105" t="s">
         <v>196</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" t="s">
         <v>236</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" t="s">
         <v>61</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="E105" t="s">
         <v>212</v>
       </c>
-      <c r="F105" s="1"/>
-      <c r="G105" s="2">
+      <c r="G105" s="1">
         <v>74</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B106" s="1" t="s">
+      <c r="A106" t="s">
+        <v>42</v>
+      </c>
+      <c r="B106" t="s">
         <v>196</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" t="s">
         <v>229</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" t="s">
         <v>230</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E106" t="s">
         <v>231</v>
       </c>
-      <c r="F106" s="1"/>
-      <c r="G106" s="2">
+      <c r="G106" s="1">
         <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B107" s="1" t="s">
+      <c r="A107" t="s">
+        <v>42</v>
+      </c>
+      <c r="B107" t="s">
         <v>196</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" t="s">
         <v>238</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" t="s">
         <v>144</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="E107" t="s">
         <v>239</v>
       </c>
-      <c r="F107" s="1" t="s">
+      <c r="F107" t="s">
         <v>240</v>
       </c>
-      <c r="G107" s="2">
+      <c r="G107" s="1">
         <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B108" s="1" t="s">
+      <c r="A108" t="s">
+        <v>42</v>
+      </c>
+      <c r="B108" t="s">
         <v>196</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" t="s">
         <v>227</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" t="s">
         <v>44</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="E108" t="s">
         <v>228</v>
       </c>
-      <c r="F108" s="1"/>
-      <c r="G108" s="2">
+      <c r="G108" s="1">
         <v>77</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>37</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" t="s">
         <v>7</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" t="s">
         <v>38</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" t="s">
         <v>39</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="E109" t="s">
         <v>40</v>
       </c>
-      <c r="F109" s="1" t="s">
+      <c r="F109" t="s">
         <v>41</v>
       </c>
-      <c r="G109" s="2">
+      <c r="G109" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>37</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C110" s="1" t="s">
+      <c r="B110" t="s">
+        <v>53</v>
+      </c>
+      <c r="C110" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" t="s">
         <v>83</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="E110" t="s">
         <v>40</v>
       </c>
-      <c r="F110" s="1"/>
-      <c r="G110" s="2">
+      <c r="G110" s="1">
         <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>37</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C111" s="1" t="s">
+      <c r="B111" t="s">
+        <v>53</v>
+      </c>
+      <c r="C111" t="s">
         <v>79</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" t="s">
         <v>80</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E111" t="s">
         <v>81</v>
       </c>
-      <c r="F111" s="1"/>
-      <c r="G111" s="2">
+      <c r="G111" s="1">
         <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>37</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C112" s="1" t="s">
+      <c r="B112" t="s">
+        <v>53</v>
+      </c>
+      <c r="C112" t="s">
         <v>87</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" t="s">
         <v>88</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="E112" t="s">
         <v>274</v>
       </c>
-      <c r="F112" s="1"/>
-      <c r="G112" s="2">
+      <c r="G112" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="A113" t="s">
         <v>37</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C113" s="3" t="s">
+      <c r="B113" t="s">
+        <v>53</v>
+      </c>
+      <c r="C113" t="s">
         <v>76</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D113" t="s">
         <v>77</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E113" t="s">
         <v>78</v>
       </c>
-      <c r="G113" s="7">
+      <c r="G113" s="5">
         <v>44</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+      <c r="A114" t="s">
         <v>37</v>
       </c>
-      <c r="B114" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C114" s="3" t="s">
+      <c r="B114" t="s">
+        <v>53</v>
+      </c>
+      <c r="C114" t="s">
+        <v>275</v>
+      </c>
+      <c r="D114" t="s">
+        <v>276</v>
+      </c>
+      <c r="E114" t="s">
+        <v>277</v>
+      </c>
+      <c r="G114" s="5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115" t="s">
+        <v>53</v>
+      </c>
+      <c r="C115" t="s">
         <v>84</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D115" t="s">
         <v>85</v>
       </c>
-      <c r="E114" s="3" t="s">
+      <c r="E115" t="s">
         <v>86</v>
       </c>
-      <c r="G114" s="7">
+      <c r="G115" s="5">
         <v>46</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>37</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" t="s">
         <v>196</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C116" t="s">
         <v>200</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D116" t="s">
         <v>201</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="E116" t="s">
         <v>202</v>
       </c>
-      <c r="G115" s="7">
+      <c r="G116" s="5">
         <v>79</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>37</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" t="s">
         <v>196</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C117" t="s">
         <v>197</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D117" t="s">
         <v>198</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="E117" t="s">
         <v>199</v>
       </c>
-      <c r="G116" s="7">
+      <c r="G117" s="5">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>37</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" t="s">
         <v>196</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" t="s">
         <v>203</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D118" t="s">
         <v>204</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E118" t="s">
         <v>205</v>
       </c>
-      <c r="G117" s="7">
+      <c r="G118" s="5">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G117"/>
-  <sortState ref="B2:H116">
-    <sortCondition ref="B2:B116" customList="High Priority,Error,Warning"/>
+  <autoFilter ref="A1:G118" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H117">
+    <sortCondition ref="B2:B117" customList="High Priority,Error,Warning"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
found duplicates in the evachecks.csv so renumbered a couple of issues
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D4594E9-6F2E-41C8-A08B-AE8416278BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB365679-0163-4759-AC48-767A852C2597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
-    <sheet name="EvaChecks (5)" sheetId="1" r:id="rId1"/>
+    <sheet name="EvaChecks (6)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1732,7 +1732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3997,19 +3999,19 @@
         <v>253</v>
       </c>
       <c r="B112" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C112" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="D112" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="E112" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="G112">
-        <v>42</v>
+        <v>128</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4017,19 +4019,19 @@
         <v>253</v>
       </c>
       <c r="B113" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="D113" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="E113" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="G113">
-        <v>110</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4040,16 +4042,16 @@
         <v>52</v>
       </c>
       <c r="C114" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D114" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E114" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="G114">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4060,16 +4062,16 @@
         <v>52</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D115" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E115" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G115">
-        <v>44</v>
+        <v>110</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4077,19 +4079,19 @@
         <v>253</v>
       </c>
       <c r="B116" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C116" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D116" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E116" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G116">
-        <v>128</v>
+        <v>43</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4097,19 +4099,19 @@
         <v>253</v>
       </c>
       <c r="B117" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C117" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D117" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E117" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G117">
-        <v>129</v>
+        <v>44</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4129,7 +4131,7 @@
         <v>277</v>
       </c>
       <c r="G118">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding VSPs participating in HMIS issue as ID 133
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB365679-0163-4759-AC48-767A852C2597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB87D530-7CDF-460F-941E-FF462DEF19D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EvaChecks (6)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="293">
   <si>
     <t>Source</t>
   </si>
@@ -890,12 +903,21 @@
   </si>
   <si>
     <t>Any project with active beds in the reporting period should have one or more active clients in the reporting period.</t>
+  </si>
+  <si>
+    <t>VSP participating in HMIS</t>
+  </si>
+  <si>
+    <t>2.08 HMIS Participation Status, 2.01 Victim Service Provider</t>
+  </si>
+  <si>
+    <t>This project is set as HMIS Participating, but the Organization it belongs to is set to Victim Service Provider = Yes. The Violence Against Women Act (VAWA) prohibits Victim Service Providers (VSPs) from entering data into HMIS and other shared databases. HUD has created this [decision tree](https://www.hudexchange.info/resource/5743/hmis-when-to-use-a-comparable-database/) to help communities and providers determine if they should enter data into HMIS or a comparable database.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1032,7 +1054,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1212,6 +1234,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1373,8 +1401,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1729,14 +1764,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="91.7109375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1751,7 +1792,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -1761,7 +1802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1774,14 +1815,14 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1794,14 +1835,14 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1814,14 +1855,14 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G4">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1834,7 +1875,7 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F5" t="s">
@@ -1844,7 +1885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1857,7 +1898,7 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F6" t="s">
@@ -1867,7 +1908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1880,14 +1921,14 @@
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G7">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1900,14 +1941,14 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G8">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1920,14 +1961,14 @@
       <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G9">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +1981,7 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F10" t="s">
@@ -1950,7 +1991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1963,14 +2004,14 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1983,14 +2024,14 @@
       <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2003,14 +2044,14 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G13">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2023,14 +2064,14 @@
       <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G14">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2043,14 +2084,14 @@
       <c r="D15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
       <c r="G15">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2063,14 +2104,14 @@
       <c r="D16" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>49</v>
       </c>
       <c r="G16">
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2083,14 +2124,14 @@
       <c r="D17" t="s">
         <v>28</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G17">
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2103,14 +2144,14 @@
       <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G18">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2123,7 +2164,7 @@
       <c r="D19" t="s">
         <v>19</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
@@ -2133,7 +2174,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2146,14 +2187,14 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G20">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2166,7 +2207,7 @@
       <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F21" t="s">
@@ -2176,7 +2217,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -2189,14 +2230,14 @@
       <c r="D22" t="s">
         <v>59</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G22">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -2209,14 +2250,14 @@
       <c r="D23" t="s">
         <v>62</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G23">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2229,14 +2270,14 @@
       <c r="D24" t="s">
         <v>65</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G24">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -2249,14 +2290,14 @@
       <c r="D25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G25">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2269,14 +2310,14 @@
       <c r="D26" t="s">
         <v>71</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G26">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -2289,14 +2330,14 @@
       <c r="D27" t="s">
         <v>74</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>75</v>
       </c>
       <c r="G27">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -2309,14 +2350,14 @@
       <c r="D28" t="s">
         <v>78</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -2329,14 +2370,14 @@
       <c r="D29" t="s">
         <v>71</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>81</v>
       </c>
       <c r="G29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2349,14 +2390,14 @@
       <c r="D30" t="s">
         <v>71</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>83</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2369,14 +2410,14 @@
       <c r="D31" t="s">
         <v>71</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>85</v>
       </c>
       <c r="G31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -2389,14 +2430,14 @@
       <c r="D32" t="s">
         <v>87</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G32">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -2409,14 +2450,14 @@
       <c r="D33" t="s">
         <v>87</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>90</v>
       </c>
       <c r="G33">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -2429,14 +2470,14 @@
       <c r="D34" t="s">
         <v>92</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G34">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -2449,14 +2490,14 @@
       <c r="D35" t="s">
         <v>92</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G35">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2469,14 +2510,14 @@
       <c r="D36" t="s">
         <v>96</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>97</v>
       </c>
       <c r="G36">
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -2489,14 +2530,14 @@
       <c r="D37" t="s">
         <v>99</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G37">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -2509,14 +2550,14 @@
       <c r="D38" t="s">
         <v>99</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G38">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2529,14 +2570,14 @@
       <c r="D39" t="s">
         <v>99</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G39">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2549,14 +2590,14 @@
       <c r="D40" t="s">
         <v>99</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>106</v>
       </c>
       <c r="G40">
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -2569,14 +2610,14 @@
       <c r="D41" t="s">
         <v>99</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G41">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -2589,14 +2630,14 @@
       <c r="D42" t="s">
         <v>110</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G42">
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -2609,14 +2650,14 @@
       <c r="D43" t="s">
         <v>110</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="2" t="s">
         <v>113</v>
       </c>
       <c r="G43">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -2629,14 +2670,14 @@
       <c r="D44" t="s">
         <v>110</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="2" t="s">
         <v>115</v>
       </c>
       <c r="G44">
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -2649,14 +2690,14 @@
       <c r="D45" t="s">
         <v>117</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="2" t="s">
         <v>118</v>
       </c>
       <c r="G45">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -2669,14 +2710,14 @@
       <c r="D46" t="s">
         <v>87</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G46">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -2689,14 +2730,14 @@
       <c r="D47" t="s">
         <v>87</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="2" t="s">
         <v>122</v>
       </c>
       <c r="G47">
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -2709,14 +2750,14 @@
       <c r="D48" t="s">
         <v>92</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G48">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -2729,14 +2770,14 @@
       <c r="D49" t="s">
         <v>92</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>122</v>
       </c>
       <c r="G49">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -2749,14 +2790,14 @@
       <c r="D50" t="s">
         <v>126</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="2" t="s">
         <v>127</v>
       </c>
       <c r="G50">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -2769,14 +2810,14 @@
       <c r="D51" t="s">
         <v>129</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="2" t="s">
         <v>130</v>
       </c>
       <c r="G51">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -2789,14 +2830,14 @@
       <c r="D52" t="s">
         <v>132</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G52">
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -2809,14 +2850,14 @@
       <c r="D53" t="s">
         <v>135</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G53">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -2829,14 +2870,14 @@
       <c r="D54" t="s">
         <v>138</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="2" t="s">
         <v>139</v>
       </c>
       <c r="G54">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -2849,14 +2890,14 @@
       <c r="D55" t="s">
         <v>141</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G55">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -2869,14 +2910,14 @@
       <c r="D56" t="s">
         <v>143</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="2" t="s">
         <v>144</v>
       </c>
       <c r="G56">
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -2889,14 +2930,14 @@
       <c r="D57" t="s">
         <v>146</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="2" t="s">
         <v>147</v>
       </c>
       <c r="G57">
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -2909,14 +2950,14 @@
       <c r="D58" t="s">
         <v>149</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G58">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -2929,14 +2970,14 @@
       <c r="D59" t="s">
         <v>151</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G59">
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>76</v>
       </c>
@@ -2949,14 +2990,14 @@
       <c r="D60" t="s">
         <v>153</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="2" t="s">
         <v>154</v>
       </c>
       <c r="G60">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -2969,14 +3010,14 @@
       <c r="D61" t="s">
         <v>156</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="2" t="s">
         <v>154</v>
       </c>
       <c r="G61">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -2989,14 +3030,14 @@
       <c r="D62" t="s">
         <v>158</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G62">
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -3009,14 +3050,14 @@
       <c r="D63" t="s">
         <v>160</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G63">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -3029,14 +3070,14 @@
       <c r="D64" t="s">
         <v>162</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G64">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -3049,14 +3090,14 @@
       <c r="D65" t="s">
         <v>164</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G65">
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -3069,14 +3110,14 @@
       <c r="D66" t="s">
         <v>166</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G66">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -3089,7 +3130,7 @@
       <c r="D67" t="s">
         <v>168</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G67">
@@ -3109,14 +3150,14 @@
       <c r="D68" t="s">
         <v>65</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="2" t="s">
         <v>170</v>
       </c>
       <c r="G68">
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -3129,14 +3170,14 @@
       <c r="D69" t="s">
         <v>172</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G69">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -3149,14 +3190,14 @@
       <c r="D70" t="s">
         <v>174</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G70">
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -3169,14 +3210,14 @@
       <c r="D71" t="s">
         <v>176</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="2" t="s">
         <v>177</v>
       </c>
       <c r="G71">
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -3189,14 +3230,14 @@
       <c r="D72" t="s">
         <v>179</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G72">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -3209,14 +3250,14 @@
       <c r="D73" t="s">
         <v>68</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G73">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -3229,14 +3270,14 @@
       <c r="D74" t="s">
         <v>182</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="2" t="s">
         <v>183</v>
       </c>
       <c r="G74">
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -3249,7 +3290,7 @@
       <c r="D75" t="s">
         <v>185</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G75">
@@ -3269,14 +3310,14 @@
       <c r="D76" t="s">
         <v>187</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="2" t="s">
         <v>170</v>
       </c>
       <c r="G76">
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -3289,14 +3330,14 @@
       <c r="D77" t="s">
         <v>189</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G77">
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -3309,14 +3350,14 @@
       <c r="D78" t="s">
         <v>132</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G78">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -3329,14 +3370,14 @@
       <c r="D79" t="s">
         <v>135</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G79">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -3349,14 +3390,14 @@
       <c r="D80" t="s">
         <v>96</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G80">
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>76</v>
       </c>
@@ -3369,14 +3410,14 @@
       <c r="D81" t="s">
         <v>194</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="2" t="s">
         <v>195</v>
       </c>
       <c r="G81">
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -3389,14 +3430,14 @@
       <c r="D82" t="s">
         <v>197</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="2" t="s">
         <v>198</v>
       </c>
       <c r="G82">
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>76</v>
       </c>
@@ -3409,14 +3450,14 @@
       <c r="D83" t="s">
         <v>201</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="2" t="s">
         <v>202</v>
       </c>
       <c r="G83">
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>76</v>
       </c>
@@ -3429,7 +3470,7 @@
       <c r="D84" t="s">
         <v>204</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="2" t="s">
         <v>205</v>
       </c>
       <c r="F84" t="s">
@@ -3439,7 +3480,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>76</v>
       </c>
@@ -3452,14 +3493,14 @@
       <c r="D85" t="s">
         <v>62</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G85">
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>76</v>
       </c>
@@ -3472,14 +3513,14 @@
       <c r="D86" t="s">
         <v>151</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G86">
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>76</v>
       </c>
@@ -3492,14 +3533,14 @@
       <c r="D87" t="s">
         <v>160</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G87">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
@@ -3512,14 +3553,14 @@
       <c r="D88" t="s">
         <v>212</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G88">
         <v>73</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -3532,14 +3573,14 @@
       <c r="D89" t="s">
         <v>126</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G89">
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>76</v>
       </c>
@@ -3552,14 +3593,14 @@
       <c r="D90" t="s">
         <v>166</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G90">
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>76</v>
       </c>
@@ -3572,14 +3613,14 @@
       <c r="D91" t="s">
         <v>168</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G91">
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>76</v>
       </c>
@@ -3592,14 +3633,14 @@
       <c r="D92" t="s">
         <v>179</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G92">
         <v>63</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>76</v>
       </c>
@@ -3612,14 +3653,14 @@
       <c r="D93" t="s">
         <v>68</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G93">
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>76</v>
       </c>
@@ -3632,14 +3673,14 @@
       <c r="D94" t="s">
         <v>219</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G94">
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>76</v>
       </c>
@@ -3652,14 +3693,14 @@
       <c r="D95" t="s">
         <v>187</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G95">
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>76</v>
       </c>
@@ -3672,14 +3713,14 @@
       <c r="D96" t="s">
         <v>189</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G96">
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>76</v>
       </c>
@@ -3692,14 +3733,14 @@
       <c r="D97" t="s">
         <v>153</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G97">
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>76</v>
       </c>
@@ -3712,7 +3753,7 @@
       <c r="D98" t="s">
         <v>110</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="2" t="s">
         <v>224</v>
       </c>
       <c r="F98" t="s">
@@ -3722,7 +3763,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>76</v>
       </c>
@@ -3735,7 +3776,7 @@
       <c r="D99" t="s">
         <v>110</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="2" t="s">
         <v>227</v>
       </c>
       <c r="F99" t="s">
@@ -3745,7 +3786,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>76</v>
       </c>
@@ -3758,14 +3799,14 @@
       <c r="D100" t="s">
         <v>229</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="2" t="s">
         <v>230</v>
       </c>
       <c r="G100">
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>76</v>
       </c>
@@ -3778,14 +3819,14 @@
       <c r="D101" t="s">
         <v>232</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="2" t="s">
         <v>233</v>
       </c>
       <c r="G101">
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>76</v>
       </c>
@@ -3798,14 +3839,14 @@
       <c r="D102" t="s">
         <v>232</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="2" t="s">
         <v>235</v>
       </c>
       <c r="G102">
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>76</v>
       </c>
@@ -3818,14 +3859,14 @@
       <c r="D103" t="s">
         <v>65</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G103">
         <v>78</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>76</v>
       </c>
@@ -3838,14 +3879,14 @@
       <c r="D104" t="s">
         <v>238</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="2" t="s">
         <v>239</v>
       </c>
       <c r="G104">
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>76</v>
       </c>
@@ -3858,14 +3899,14 @@
       <c r="D105" t="s">
         <v>229</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G105">
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>76</v>
       </c>
@@ -3878,7 +3919,7 @@
       <c r="D106" t="s">
         <v>229</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E106" s="2" t="s">
         <v>243</v>
       </c>
       <c r="F106" t="s">
@@ -3888,7 +3929,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>76</v>
       </c>
@@ -3901,14 +3942,14 @@
       <c r="D107" t="s">
         <v>62</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="2" t="s">
         <v>208</v>
       </c>
       <c r="G107">
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>76</v>
       </c>
@@ -3921,14 +3962,14 @@
       <c r="D108" t="s">
         <v>232</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="2" t="s">
         <v>247</v>
       </c>
       <c r="G108">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>76</v>
       </c>
@@ -3941,7 +3982,7 @@
       <c r="D109" t="s">
         <v>138</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="2" t="s">
         <v>249</v>
       </c>
       <c r="F109" t="s">
@@ -3951,7 +3992,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>76</v>
       </c>
@@ -3964,7 +4005,7 @@
       <c r="D110" t="s">
         <v>78</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="2" t="s">
         <v>252</v>
       </c>
       <c r="G110">
@@ -3984,7 +4025,7 @@
       <c r="D111" t="s">
         <v>255</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="2" t="s">
         <v>256</v>
       </c>
       <c r="F111" t="s">
@@ -3994,7 +4035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>253</v>
       </c>
@@ -4007,14 +4048,14 @@
       <c r="D112" t="s">
         <v>270</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="2" t="s">
         <v>271</v>
       </c>
       <c r="G112">
         <v>128</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>253</v>
       </c>
@@ -4027,7 +4068,7 @@
       <c r="D113" t="s">
         <v>273</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="2" t="s">
         <v>274</v>
       </c>
       <c r="G113">
@@ -4047,7 +4088,7 @@
       <c r="D114" t="s">
         <v>259</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="2" t="s">
         <v>256</v>
       </c>
       <c r="G114">
@@ -4067,7 +4108,7 @@
       <c r="D115" t="s">
         <v>261</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="2" t="s">
         <v>262</v>
       </c>
       <c r="G115">
@@ -4087,14 +4128,14 @@
       <c r="D116" t="s">
         <v>264</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="2" t="s">
         <v>265</v>
       </c>
       <c r="G116">
         <v>43</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>253</v>
       </c>
@@ -4107,14 +4148,14 @@
       <c r="D117" t="s">
         <v>267</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="2" t="s">
         <v>268</v>
       </c>
       <c r="G117">
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>253</v>
       </c>
@@ -4127,54 +4168,55 @@
       <c r="D118" t="s">
         <v>276</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G118">
         <v>132</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="119" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B119" t="s">
-        <v>52</v>
-      </c>
-      <c r="C119" t="s">
-        <v>278</v>
-      </c>
-      <c r="D119" t="s">
-        <v>279</v>
-      </c>
-      <c r="E119" t="s">
-        <v>280</v>
-      </c>
-      <c r="G119">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>253</v>
       </c>
       <c r="B120" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="C120" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D120" t="s">
-        <v>282</v>
-      </c>
-      <c r="E120" t="s">
-        <v>283</v>
+        <v>279</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="G120">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>253</v>
       </c>
@@ -4182,19 +4224,19 @@
         <v>199</v>
       </c>
       <c r="C121" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D121" t="s">
-        <v>285</v>
-      </c>
-      <c r="E121" t="s">
-        <v>286</v>
+        <v>282</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="G121">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>253</v>
       </c>
@@ -4202,15 +4244,35 @@
         <v>199</v>
       </c>
       <c r="C122" t="s">
+        <v>284</v>
+      </c>
+      <c r="D122" t="s">
+        <v>285</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G122">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>253</v>
+      </c>
+      <c r="B123" t="s">
+        <v>199</v>
+      </c>
+      <c r="C123" t="s">
         <v>287</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D123" t="s">
         <v>288</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E123" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G122">
+      <c r="G123">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change text for Don't Know =Doesn't Know and Refused = Prefers Not to Answer
</commit_message>
<xml_diff>
--- a/public-resources/EvaChecks.xlsx
+++ b/public-resources/EvaChecks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denzing\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\eva\public-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB87D530-7CDF-460F-941E-FF462DEF19D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A548990A-9181-4AB3-AEF3-1A12BB1E17B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EvaChecks (6)" sheetId="1" r:id="rId1"/>
@@ -656,54 +656,15 @@
     <t>Includes ES-NbN, Street Outreach, and Coordinated Entry</t>
   </si>
   <si>
-    <t>Don't Know/Refused Destination</t>
-  </si>
-  <si>
     <t>This record is being flagged because it is incomplete. Some clients may decline or be unable to provide the answer to one or more questions during an assessment. Please review the HMIS Data Manual, pages 12-13, for further guidance on data completeness. If possible to complete this data, please update the record. Note that high levels of incomplete data for a given element may indicate the need for additional training.</t>
   </si>
   <si>
-    <t>Don't Know/Refused Discharge Status</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused Gender</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused Length of Stay</t>
-  </si>
-  <si>
     <t>3.917.2 - Length of Stay in prior living situation</t>
   </si>
   <si>
-    <t>Don't Know/Refused Living Situation</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused Military Branch</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused Months or Times Homeless</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused Race/Ethnicity</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused Residence Prior</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused SSN</t>
-  </si>
-  <si>
     <t>3.02 - Social Security Number</t>
   </si>
   <si>
-    <t>Don't Know/Refused Veteran Status</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused War(s)</t>
-  </si>
-  <si>
-    <t>Don't Know/Refused/Data Not Collected DOB</t>
-  </si>
-  <si>
     <t>Enrollment After Participating Period</t>
   </si>
   <si>
@@ -743,9 +704,6 @@
     <t>This client has an Approximate Date Homelessness Started in their enrollment that is after their Project Start Date. The information at Project Start should reflect the client's situation at the point of Project Start, so this date may have been incorrectly entered.</t>
   </si>
   <si>
-    <t>Incomplete or Don't Know/Refused Name</t>
-  </si>
-  <si>
     <t>Invalid Homelessness Start Date/Number of Months Homeless</t>
   </si>
   <si>
@@ -912,6 +870,48 @@
   </si>
   <si>
     <t>This project is set as HMIS Participating, but the Organization it belongs to is set to Victim Service Provider = Yes. The Violence Against Women Act (VAWA) prohibits Victim Service Providers (VSPs) from entering data into HMIS and other shared databases. HUD has created this [decision tree](https://www.hudexchange.info/resource/5743/hmis-when-to-use-a-comparable-database/) to help communities and providers determine if they should enter data into HMIS or a comparable database.</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Destination</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Discharge Status</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Gender</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Length of Stay</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Living Situation</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Military Branch</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Months or Times Homeless</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Race/Ethnicity</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Residence Prior</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer SSN</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer Veteran Status</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer War(s)</t>
+  </si>
+  <si>
+    <t>Doesn't Know/Prefers Not to Answer/Data Not Collected DOB</t>
+  </si>
+  <si>
+    <t>Incomplete or Doesn't Know/Prefers Not to Answer Name</t>
   </si>
 </sst>
 </file>
@@ -1768,7 +1768,7 @@
   <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
@@ -3488,13 +3488,13 @@
         <v>199</v>
       </c>
       <c r="C85" t="s">
-        <v>207</v>
+        <v>279</v>
       </c>
       <c r="D85" t="s">
         <v>62</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G85">
         <v>59</v>
@@ -3508,13 +3508,13 @@
         <v>199</v>
       </c>
       <c r="C86" t="s">
-        <v>209</v>
+        <v>280</v>
       </c>
       <c r="D86" t="s">
         <v>151</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G86">
         <v>56</v>
@@ -3528,13 +3528,13 @@
         <v>199</v>
       </c>
       <c r="C87" t="s">
-        <v>210</v>
+        <v>281</v>
       </c>
       <c r="D87" t="s">
         <v>160</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G87">
         <v>65</v>
@@ -3548,13 +3548,13 @@
         <v>199</v>
       </c>
       <c r="C88" t="s">
-        <v>211</v>
+        <v>282</v>
       </c>
       <c r="D88" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G88">
         <v>73</v>
@@ -3568,13 +3568,13 @@
         <v>199</v>
       </c>
       <c r="C89" t="s">
-        <v>213</v>
+        <v>283</v>
       </c>
       <c r="D89" t="s">
         <v>126</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G89">
         <v>68</v>
@@ -3588,13 +3588,13 @@
         <v>199</v>
       </c>
       <c r="C90" t="s">
-        <v>214</v>
+        <v>284</v>
       </c>
       <c r="D90" t="s">
         <v>166</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G90">
         <v>58</v>
@@ -3608,13 +3608,13 @@
         <v>199</v>
       </c>
       <c r="C91" t="s">
-        <v>215</v>
+        <v>285</v>
       </c>
       <c r="D91" t="s">
         <v>168</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G91">
         <v>61</v>
@@ -3628,13 +3628,13 @@
         <v>199</v>
       </c>
       <c r="C92" t="s">
-        <v>216</v>
+        <v>286</v>
       </c>
       <c r="D92" t="s">
         <v>179</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G92">
         <v>63</v>
@@ -3648,13 +3648,13 @@
         <v>199</v>
       </c>
       <c r="C93" t="s">
-        <v>217</v>
+        <v>287</v>
       </c>
       <c r="D93" t="s">
         <v>68</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G93">
         <v>64</v>
@@ -3668,13 +3668,13 @@
         <v>199</v>
       </c>
       <c r="C94" t="s">
-        <v>218</v>
+        <v>288</v>
       </c>
       <c r="D94" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G94">
         <v>67</v>
@@ -3688,13 +3688,13 @@
         <v>199</v>
       </c>
       <c r="C95" t="s">
-        <v>220</v>
+        <v>289</v>
       </c>
       <c r="D95" t="s">
         <v>187</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G95">
         <v>66</v>
@@ -3708,13 +3708,13 @@
         <v>199</v>
       </c>
       <c r="C96" t="s">
-        <v>221</v>
+        <v>290</v>
       </c>
       <c r="D96" t="s">
         <v>189</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G96">
         <v>57</v>
@@ -3728,13 +3728,13 @@
         <v>199</v>
       </c>
       <c r="C97" t="s">
-        <v>222</v>
+        <v>291</v>
       </c>
       <c r="D97" t="s">
         <v>153</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G97">
         <v>60</v>
@@ -3748,16 +3748,16 @@
         <v>199</v>
       </c>
       <c r="C98" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D98" t="s">
         <v>110</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F98" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="G98">
         <v>111</v>
@@ -3771,16 +3771,16 @@
         <v>199</v>
       </c>
       <c r="C99" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D99" t="s">
         <v>110</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="F99" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="G99">
         <v>113</v>
@@ -3794,13 +3794,13 @@
         <v>199</v>
       </c>
       <c r="C100" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="D100" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="G100">
         <v>75</v>
@@ -3814,13 +3814,13 @@
         <v>199</v>
       </c>
       <c r="C101" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="D101" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="G101">
         <v>105</v>
@@ -3834,13 +3834,13 @@
         <v>199</v>
       </c>
       <c r="C102" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D102" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="G102">
         <v>69</v>
@@ -3854,13 +3854,13 @@
         <v>199</v>
       </c>
       <c r="C103" t="s">
-        <v>236</v>
+        <v>292</v>
       </c>
       <c r="D103" t="s">
         <v>65</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G103">
         <v>78</v>
@@ -3874,13 +3874,13 @@
         <v>199</v>
       </c>
       <c r="C104" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="D104" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="G104">
         <v>71</v>
@@ -3894,13 +3894,13 @@
         <v>199</v>
       </c>
       <c r="C105" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="D105" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G105">
         <v>102</v>
@@ -3914,16 +3914,16 @@
         <v>199</v>
       </c>
       <c r="C106" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="D106" t="s">
+        <v>216</v>
+      </c>
+      <c r="E106" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E106" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="F106" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G106">
         <v>104</v>
@@ -3937,13 +3937,13 @@
         <v>199</v>
       </c>
       <c r="C107" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="D107" t="s">
         <v>62</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G107">
         <v>74</v>
@@ -3957,13 +3957,13 @@
         <v>199</v>
       </c>
       <c r="C108" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="D108" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="G108">
         <v>70</v>
@@ -3977,16 +3977,16 @@
         <v>199</v>
       </c>
       <c r="C109" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="D109" t="s">
         <v>138</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="F109" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="G109">
         <v>72</v>
@@ -4000,13 +4000,13 @@
         <v>199</v>
       </c>
       <c r="C110" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D110" t="s">
         <v>78</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="G110">
         <v>77</v>
@@ -4014,22 +4014,22 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B111" t="s">
         <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="D111" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="F111" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="G111">
         <v>5</v>
@@ -4037,19 +4037,19 @@
     </row>
     <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
       </c>
       <c r="C112" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="D112" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="G112">
         <v>128</v>
@@ -4057,19 +4057,19 @@
     </row>
     <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B113" t="s">
         <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="D113" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="G113">
         <v>131</v>
@@ -4077,19 +4077,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B114" t="s">
         <v>52</v>
       </c>
       <c r="C114" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="D114" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="G114">
         <v>42</v>
@@ -4097,19 +4097,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B115" t="s">
         <v>52</v>
       </c>
       <c r="C115" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="D115" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="G115">
         <v>110</v>
@@ -4117,19 +4117,19 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B116" t="s">
         <v>52</v>
       </c>
       <c r="C116" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="D116" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="G116">
         <v>43</v>
@@ -4137,19 +4137,19 @@
     </row>
     <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>239</v>
+      </c>
+      <c r="B117" t="s">
+        <v>52</v>
+      </c>
+      <c r="C117" t="s">
+        <v>252</v>
+      </c>
+      <c r="D117" t="s">
         <v>253</v>
       </c>
-      <c r="B117" t="s">
-        <v>52</v>
-      </c>
-      <c r="C117" t="s">
-        <v>266</v>
-      </c>
-      <c r="D117" t="s">
-        <v>267</v>
-      </c>
       <c r="E117" s="2" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="G117">
         <v>44</v>
@@ -4157,19 +4157,19 @@
     </row>
     <row r="118" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B118" t="s">
         <v>52</v>
       </c>
       <c r="C118" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="D118" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="G118">
         <v>132</v>
@@ -4177,19 +4177,19 @@
     </row>
     <row r="119" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1">
@@ -4198,19 +4198,19 @@
     </row>
     <row r="120" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B120" t="s">
         <v>52</v>
       </c>
       <c r="C120" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="D120" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="G120">
         <v>46</v>
@@ -4218,19 +4218,19 @@
     </row>
     <row r="121" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B121" t="s">
         <v>199</v>
       </c>
       <c r="C121" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="D121" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="G121">
         <v>79</v>
@@ -4238,19 +4238,19 @@
     </row>
     <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B122" t="s">
         <v>199</v>
       </c>
       <c r="C122" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="D122" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="G122">
         <v>81</v>
@@ -4258,19 +4258,19 @@
     </row>
     <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B123" t="s">
         <v>199</v>
       </c>
       <c r="C123" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="D123" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="G123">
         <v>83</v>

</xml_diff>